<commit_message>
Increased delay for SMCU startup Added start points from FW to trajectory calculator
</commit_message>
<xml_diff>
--- a/docs/IK and trajectory algorithms.xlsx
+++ b/docs/IK and trajectory algorithms.xlsx
@@ -1223,6 +1223,117 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1283,18 +1394,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1302,105 +1401,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1528,67 +1528,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-23.82813296867765</c:v>
+                  <c:v>-100.14892496555947</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-23.519433521775909</c:v>
+                  <c:v>-101.79746874221689</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-23.19375952853526</c:v>
+                  <c:v>-103.41111038876282</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-22.851284810475221</c:v>
+                  <c:v>-104.98929686774301</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-22.492192156142416</c:v>
+                  <c:v>-106.53148729312204</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-22.116673223551054</c:v>
+                  <c:v>-108.03715311565934</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-21.724928437889609</c:v>
+                  <c:v>-109.50577830405679</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-21.317166884548143</c:v>
+                  <c:v>-110.93685952181639</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-20.893606197523482</c:v>
+                  <c:v>-112.32990629974668</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-20.454472443261693</c:v>
+                  <c:v>-113.68444120405972</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-20</c:v>
+                  <c:v>-115</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-19.53043143267238</c:v>
+                  <c:v>-116.27613181094999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-19.046017363445763</c:v>
+                  <c:v>-117.51239927295748</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-18.547016337955782</c:v>
+                  <c:v>-118.70837868463155</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-18.033694687313591</c:v>
+                  <c:v>-119.86366015235637</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-17.506326385957379</c:v>
+                  <c:v>-120.97784773077237</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-16.965192905424296</c:v>
+                  <c:v>-122.05055955847723</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-16.410583064121127</c:v>
+                  <c:v>-123.08142798889988</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-15.842792873173584</c:v>
+                  <c:v>-124.07009971630248</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-15.262125378436776</c:v>
+                  <c:v>-125.01623589686776</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-14.668890498750928</c:v>
+                  <c:v>-125.91951226482961</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1600,67 +1600,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>12.992055089910252</c:v>
+                  <c:v>89.979771222137614</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.730417435430004</c:v>
+                  <c:v>88.109660550196153</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.461451464682787</c:v>
+                  <c:v>86.209352379030832</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.184767003910704</c:v>
+                  <c:v>84.279497994257369</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.899977998934611</c:v>
+                  <c:v>82.32075880775642</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.606702721202282</c:v>
+                  <c:v>80.33380613099024</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.304563971527834</c:v>
+                  <c:v>78.319320944926616</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17.993189281413734</c:v>
+                  <c:v>76.277993666648783</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.67221111184783</c:v>
+                  <c:v>74.210523912731404</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.341267049469508</c:v>
+                  <c:v>72.117620259463308</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.000000000000004</c:v>
+                  <c:v>70.000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.648058378833856</c:v>
+                  <c:v>67.858388898528361</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21.285096298689638</c:v>
+                  <c:v>65.693520941528021</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.910773754219893</c:v>
+                  <c:v>63.506138086215103</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.524756803481743</c:v>
+                  <c:v>61.296990006253715</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23.126717746171163</c:v>
+                  <c:v>59.066833834823406</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.716335298526101</c:v>
+                  <c:v>56.816433905129294</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24.293294764804742</c:v>
+                  <c:v>54.546561488445221</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>24.857288205247652</c:v>
+                  <c:v>52.257994529778742</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25.408014600434004</c:v>
+                  <c:v>49.951517381248848</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25.945180011944267</c:v>
+                  <c:v>47.62792053326794</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1680,67 +1680,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-33.849974896909735</c:v>
+                  <c:v>-132.69246029453819</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-34.067691463555342</c:v>
+                  <c:v>-133.12987773832018</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-34.26280357707833</c:v>
+                  <c:v>-133.52165461093401</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-34.435207100566458</c:v>
+                  <c:v>-133.86765664013609</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-34.584810017331122</c:v>
+                  <c:v>-134.16776524192616</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-34.711532480019251</c:v>
+                  <c:v>-134.42187756118923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-34.81530685323019</c:v>
+                  <c:v>-134.62990650694664</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-34.896077749614562</c:v>
+                  <c:v>-134.79178078220454</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-34.953802059436164</c:v>
+                  <c:v>-134.90744490838915</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-34.988448973580795</c:v>
+                  <c:v>-134.97685924436081</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-35</c:v>
+                  <c:v>-135</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-34.988448973580795</c:v>
+                  <c:v>-134.97685924436081</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-34.953802059436164</c:v>
+                  <c:v>-134.90744490838915</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-34.896077749614562</c:v>
+                  <c:v>-134.79178078220454</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-34.81530685323019</c:v>
+                  <c:v>-134.62990650694664</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-34.711532480019251</c:v>
+                  <c:v>-134.42187756118923</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-34.584810017331115</c:v>
+                  <c:v>-134.16776524192619</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-34.435207100566458</c:v>
+                  <c:v>-133.86765664013612</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-34.26280357707833</c:v>
+                  <c:v>-133.52165461093401</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-34.067691463555342</c:v>
+                  <c:v>-133.12987773832018</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-33.849974896909728</c:v>
+                  <c:v>-132.69246029453819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1752,67 +1752,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-9.9112783872395216</c:v>
+                  <c:v>24.857437815759159</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-8.9352891362541698</c:v>
+                  <c:v>22.396038320852366</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-7.9545308660430551</c:v>
+                  <c:v>19.926963114274585</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-6.9695270353298016</c:v>
+                  <c:v>17.451058413071362</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-5.9808033688150299</c:v>
+                  <c:v>14.969172774935751</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.9888875765820613</c:v>
+                  <c:v>12.482156807385293</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.9943090724429551</c:v>
+                  <c:v>9.9908628762364113</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-2.9975986913752113</c:v>
+                  <c:v>7.4961448134761683</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.9992884062000433</c:v>
+                  <c:v>4.9988576246318139</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.99991104365316275</c:v>
+                  <c:v>2.4998571957375324</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.3029658040673552E-15</c:v>
+                  <c:v>1.6544315288987496E-14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.99991104365317329</c:v>
+                  <c:v>-2.4998571957374991</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.9992884062000542</c:v>
+                  <c:v>-4.9988576246317802</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.9975986913752215</c:v>
+                  <c:v>-7.4961448134761355</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.9943090724429466</c:v>
+                  <c:v>-9.990862876236319</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.9888875765820719</c:v>
+                  <c:v>-12.482156807385259</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.9808033688150415</c:v>
+                  <c:v>-14.96917277493572</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.9695270353298122</c:v>
+                  <c:v>-17.451058413071326</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.9545308660430658</c:v>
+                  <c:v>-19.926963114274553</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.9352891362541804</c:v>
+                  <c:v>-22.39603832085233</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.9112783872395323</c:v>
+                  <c:v>-24.857437815759127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1832,67 +1832,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-14.668890498750928</c:v>
+                  <c:v>-125.91951226482961</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-15.262125378436776</c:v>
+                  <c:v>-125.01623589686776</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-15.842792873173584</c:v>
+                  <c:v>-124.07009971630248</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-16.410583064121127</c:v>
+                  <c:v>-123.08142798889988</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-16.965192905424296</c:v>
+                  <c:v>-122.05055955847723</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-17.506326385957379</c:v>
+                  <c:v>-120.97784773077237</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-18.033694687313591</c:v>
+                  <c:v>-119.86366015235637</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-18.547016337955782</c:v>
+                  <c:v>-118.70837868463155</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-19.046017363445763</c:v>
+                  <c:v>-117.51239927295748</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-19.53043143267238</c:v>
+                  <c:v>-116.27613181094999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-20</c:v>
+                  <c:v>-115</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-20.454472443261693</c:v>
+                  <c:v>-113.68444120405972</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-20.893606197523482</c:v>
+                  <c:v>-112.32990629974668</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-21.317166884548143</c:v>
+                  <c:v>-110.93685952181639</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-21.724928437889609</c:v>
+                  <c:v>-109.50577830405679</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-22.116673223551054</c:v>
+                  <c:v>-108.03715311565934</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-22.492192156142416</c:v>
+                  <c:v>-106.53148729312204</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-22.851284810475221</c:v>
+                  <c:v>-104.98929686774301</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-23.19375952853526</c:v>
+                  <c:v>-103.41111038876282</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-23.519433521775909</c:v>
+                  <c:v>-101.79746874221689</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-23.82813296867765</c:v>
+                  <c:v>-100.14892496555947</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1904,67 +1904,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-25.945180011944267</c:v>
+                  <c:v>-47.62792053326794</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-25.408014600434004</c:v>
+                  <c:v>-49.951517381248848</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-24.857288205247652</c:v>
+                  <c:v>-52.257994529778742</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-24.293294764804742</c:v>
+                  <c:v>-54.546561488445221</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-23.716335298526101</c:v>
+                  <c:v>-56.816433905129294</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-23.126717746171163</c:v>
+                  <c:v>-59.066833834823406</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-22.524756803481743</c:v>
+                  <c:v>-61.296990006253715</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-21.910773754219893</c:v>
+                  <c:v>-63.506138086215103</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-21.285096298689638</c:v>
+                  <c:v>-65.693520941528021</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-20.648058378833856</c:v>
+                  <c:v>-67.858388898528361</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-20.000000000000004</c:v>
+                  <c:v>-70.000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-19.341267049469508</c:v>
+                  <c:v>-72.117620259463308</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-18.67221111184783</c:v>
+                  <c:v>-74.210523912731404</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-17.993189281413734</c:v>
+                  <c:v>-76.277993666648783</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-17.304563971527834</c:v>
+                  <c:v>-78.319320944926616</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-16.606702721202282</c:v>
+                  <c:v>-80.33380613099024</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-15.899977998934611</c:v>
+                  <c:v>-82.32075880775642</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-15.184767003910704</c:v>
+                  <c:v>-84.279497994257369</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-14.461451464682787</c:v>
+                  <c:v>-86.209352379030832</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-13.730417435430004</c:v>
+                  <c:v>-88.109660550196153</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-12.992055089910252</c:v>
+                  <c:v>-89.979771222137614</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1984,67 +1984,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>24.268344603103579</c:v>
+                  <c:v>125.92085434689243</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.876306657427222</c:v>
+                  <c:v>125.01732357372842</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.475946796756844</c:v>
+                  <c:v>124.07095953285281</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.067478704594315</c:v>
+                  <c:v>123.08208656812548</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.6511203920364</c:v>
+                  <c:v>122.05104359233296</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.227094081416055</c:v>
+                  <c:v>120.9781839710344</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.795626087695972</c:v>
+                  <c:v>119.86387540145367</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.356946697677845</c:v>
+                  <c:v>118.70849978645992</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.911290047091697</c:v>
+                  <c:v>117.51245310367943</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.458893995630973</c:v>
+                  <c:v>116.27614526978367</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.53485298504166</c:v>
+                  <c:v>113.68445466289337</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19.063701213013974</c:v>
+                  <c:v>112.32996013046863</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18.586796151085473</c:v>
+                  <c:v>110.93698062364474</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18.104392337119965</c:v>
+                  <c:v>109.50599355315411</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.616747243822388</c:v>
+                  <c:v>108.03748935592138</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.124121141318291</c:v>
+                  <c:v>106.53197132697777</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16.626776958240217</c:v>
+                  <c:v>104.98995544696859</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16.124980141395174</c:v>
+                  <c:v>103.41197020531315</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15.618998514088089</c:v>
+                  <c:v>101.79855641907753</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>15.109102133176851</c:v>
+                  <c:v>100.15026704762228</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2056,67 +2056,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-16.785937542017532</c:v>
+                  <c:v>47.642377801908076</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-17.150706457094863</c:v>
+                  <c:v>49.964543081841143</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-17.506321549885975</c:v>
+                  <c:v>52.26958419807282</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-17.852593018450641</c:v>
+                  <c:v>54.556711152356797</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-18.189336047807984</c:v>
+                  <c:v>56.825140086101463</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-18.516370908577485</c:v>
+                  <c:v>59.074093549018841</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-18.833523052905722</c:v>
+                  <c:v>61.302800765577338</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-19.140623207627524</c:v>
+                  <c:v>63.510497899166715</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-19.437507464611908</c:v>
+                  <c:v>65.696428313885079</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-19.724017368244535</c:v>
+                  <c:v>67.859842833857826</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-20</c:v>
+                  <c:v>70.000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-20.265308060058818</c:v>
+                  <c:v>72.116166324133829</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-20.519799945925545</c:v>
+                  <c:v>74.207616540374318</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-20.763339828006092</c:v>
+                  <c:v>76.273633853697149</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-20.995797722103841</c:v>
+                  <c:v>78.313510185602979</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-21.217049558795946</c:v>
+                  <c:v>80.326546416794784</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-21.426977249652715</c:v>
+                  <c:v>82.312052626784237</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-21.625468750264794</c:v>
+                  <c:v>84.269348330345778</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-21.812418120044455</c:v>
+                  <c:v>86.197762710736725</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-21.98772557876913</c:v>
+                  <c:v>88.096634849603845</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-22.151297559836966</c:v>
+                  <c:v>89.965313953497443</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2136,67 +2136,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>34.29018653133565</c:v>
+                  <c:v>132.69380237660101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.424564599206647</c:v>
+                  <c:v>133.13096541518081</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.544990845299921</c:v>
+                  <c:v>133.52251442748434</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.651400994685552</c:v>
+                  <c:v>133.86831521936168</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34.743738253225104</c:v>
+                  <c:v>134.1682492757819</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.821953337884253</c:v>
+                  <c:v>134.42221380145125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.886004503036553</c:v>
+                  <c:v>134.63012175604393</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34.93585756274426</c:v>
+                  <c:v>134.79190188403288</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34.971485909004379</c:v>
+                  <c:v>134.90749873911111</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.992870525950067</c:v>
+                  <c:v>134.97687270319446</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.992870525950067</c:v>
+                  <c:v>134.97687270319446</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.971485909004379</c:v>
+                  <c:v>134.90749873911111</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34.93585756274426</c:v>
+                  <c:v>134.79190188403288</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>34.886004503036553</c:v>
+                  <c:v>134.63012175604393</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>34.821953337884253</c:v>
+                  <c:v>134.42221380145125</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>34.743738253225104</c:v>
+                  <c:v>134.1682492757819</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>34.651400994685552</c:v>
+                  <c:v>133.86831521936168</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>34.544990845299921</c:v>
+                  <c:v>133.52251442748434</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34.424564599206647</c:v>
+                  <c:v>133.13096541518081</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>34.29018653133565</c:v>
+                  <c:v>132.69380237660101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2208,67 +2208,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>6.1173959351322393</c:v>
+                  <c:v>-24.842980547118994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5150001145893084</c:v>
+                  <c:v>-22.383012620260054</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.909660780839868</c:v>
+                  <c:v>-19.915373445980478</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3017010207898609</c:v>
+                  <c:v>-17.440908749159757</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.6914453199416575</c:v>
+                  <c:v>-14.960466593963559</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0792193892068549</c:v>
+                  <c:v>-12.474897093189828</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4653499910650627</c:v>
+                  <c:v>-9.9850521169127635</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8501647651614226</c:v>
+                  <c:v>-7.4917850005245246</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2339920534359656</c:v>
+                  <c:v>-4.9959502522747368</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.61716072487813445</c:v>
+                  <c:v>-2.4984032604080371</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.61716072487813523</c:v>
+                  <c:v>2.4984032604080402</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1.2339920534359656</c:v>
+                  <c:v>4.9959502522747368</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-1.8501647651614226</c:v>
+                  <c:v>7.4917850005245246</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-2.4653499910650618</c:v>
+                  <c:v>9.98505211691276</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-3.0792193892068549</c:v>
+                  <c:v>12.474897093189828</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-3.6914453199416584</c:v>
+                  <c:v>14.960466593963563</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-4.3017010207898609</c:v>
+                  <c:v>17.440908749159757</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-4.909660780839868</c:v>
+                  <c:v>19.915373445980478</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-5.5150001145893075</c:v>
+                  <c:v>22.383012620260047</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-6.1173959351322393</c:v>
+                  <c:v>24.842980547118994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2288,67 +2288,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>15.109102133176851</c:v>
+                  <c:v>100.15026704762228</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.618998514088089</c:v>
+                  <c:v>101.79855641907753</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.124980141395174</c:v>
+                  <c:v>103.41197020531315</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.626776958240217</c:v>
+                  <c:v>104.98995544696859</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.124121141318291</c:v>
+                  <c:v>106.53197132697777</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.616747243822388</c:v>
+                  <c:v>108.03748935592138</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.104392337119965</c:v>
+                  <c:v>109.50599355315411</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.586796151085473</c:v>
+                  <c:v>110.93698062364474</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19.063701213013974</c:v>
+                  <c:v>112.32996013046863</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.53485298504166</c:v>
+                  <c:v>113.68445466289337</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.458893995630973</c:v>
+                  <c:v>116.27614526978367</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.911290047091697</c:v>
+                  <c:v>117.51245310367943</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.356946697677845</c:v>
+                  <c:v>118.70849978645992</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.795626087695972</c:v>
+                  <c:v>119.86387540145367</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.227094081416055</c:v>
+                  <c:v>120.9781839710344</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22.651120392036404</c:v>
+                  <c:v>122.05104359233296</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23.067478704594315</c:v>
+                  <c:v>123.08208656812548</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>23.475946796756844</c:v>
+                  <c:v>124.07095953285281</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>23.876306657427222</c:v>
+                  <c:v>125.01732357372842</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>24.268344603103579</c:v>
+                  <c:v>125.92085434689243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2360,67 +2360,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>22.151297559836966</c:v>
+                  <c:v>-89.965313953497443</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.98772557876913</c:v>
+                  <c:v>-88.096634849603845</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.812418120044455</c:v>
+                  <c:v>-86.197762710736725</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.625468750264794</c:v>
+                  <c:v>-84.269348330345778</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.426977249652715</c:v>
+                  <c:v>-82.312052626784237</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.217049558795946</c:v>
+                  <c:v>-80.326546416794784</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.995797722103841</c:v>
+                  <c:v>-78.313510185602979</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.763339828006092</c:v>
+                  <c:v>-76.273633853697149</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.519799945925545</c:v>
+                  <c:v>-74.207616540374318</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.265308060058818</c:v>
+                  <c:v>-72.116166324133829</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>-70.000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.724017368244535</c:v>
+                  <c:v>-67.859842833857826</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19.437507464611908</c:v>
+                  <c:v>-65.696428313885079</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19.140623207627524</c:v>
+                  <c:v>-63.510497899166715</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18.833523052905722</c:v>
+                  <c:v>-61.302800765577338</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.516370908577485</c:v>
+                  <c:v>-59.074093549018841</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>18.189336047807981</c:v>
+                  <c:v>-56.825140086101456</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.852593018450641</c:v>
+                  <c:v>-54.556711152356797</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17.506321549885975</c:v>
+                  <c:v>-52.26958419807282</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17.150706457094863</c:v>
+                  <c:v>-49.964543081841143</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>16.785937542017532</c:v>
+                  <c:v>-47.642377801908076</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2440,7 +2440,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8.2842712474619002</c:v>
+                  <c:v>3.9269916244421305E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2482,40 +2482,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>8.2842712474619002</c:v>
+                  <c:v>3.9269916244421305E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-20</c:v>
+                  <c:v>-115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.2842712474619002</c:v>
+                  <c:v>3.9269916244421305E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-35</c:v>
+                  <c:v>-135</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.2842712474619002</c:v>
+                  <c:v>3.9269916244421305E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-20</c:v>
+                  <c:v>-115</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.2842712474619002</c:v>
+                  <c:v>3.9269916244421305E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.2842712474619002</c:v>
+                  <c:v>3.9269916244421305E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>35</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.2842712474619002</c:v>
+                  <c:v>3.9269916244421305E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2530,7 +2530,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2542,13 +2542,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-20</c:v>
+                  <c:v>-70</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-20</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2560,7 +2560,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20</c:v>
+                  <c:v>-70</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2575,15 +2575,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="204717056"/>
-        <c:axId val="205456128"/>
+        <c:axId val="202566656"/>
+        <c:axId val="203240192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="204717056"/>
+        <c:axId val="202566656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="50"/>
-          <c:min val="-50"/>
+          <c:max val="150"/>
+          <c:min val="-150"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2610,17 +2610,17 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205456128"/>
+        <c:crossAx val="203240192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
+        <c:majorUnit val="25"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="205456128"/>
+        <c:axId val="203240192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="50"/>
-          <c:min val="-50"/>
+          <c:max val="150"/>
+          <c:min val="-150"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2656,10 +2656,10 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204717056"/>
+        <c:crossAx val="202566656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
+        <c:majorUnit val="25"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2840,11 +2840,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="177076864"/>
-        <c:axId val="205464704"/>
+        <c:axId val="175524480"/>
+        <c:axId val="203244672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="177076864"/>
+        <c:axId val="175524480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2853,12 +2853,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205464704"/>
+        <c:crossAx val="203244672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="205464704"/>
+        <c:axId val="203244672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2869,7 +2869,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="177076864"/>
+        <c:crossAx val="175524480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3561,7 +3561,7 @@
   <dimension ref="A1:AB52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3598,14 +3598,14 @@
       <c r="AB1" s="59"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="140" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="107">
-        <v>1.5</v>
-      </c>
-      <c r="E2" s="108"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="144">
+        <v>1.9990000000000001</v>
+      </c>
+      <c r="E2" s="145"/>
       <c r="O2" s="59"/>
       <c r="P2" s="59"/>
       <c r="Q2" s="59"/>
@@ -3622,14 +3622,14 @@
       <c r="AB2" s="59"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="142" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="109">
-        <v>-20</v>
-      </c>
-      <c r="E3" s="110"/>
+      <c r="C3" s="143"/>
+      <c r="D3" s="146">
+        <v>50</v>
+      </c>
+      <c r="E3" s="147"/>
       <c r="O3" s="59"/>
       <c r="P3" s="59"/>
       <c r="Q3" s="59"/>
@@ -3662,20 +3662,20 @@
       <c r="AB4" s="59"/>
     </row>
     <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="152" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="116"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="116"/>
-      <c r="M5" s="117"/>
+      <c r="C5" s="153"/>
+      <c r="D5" s="153"/>
+      <c r="E5" s="153"/>
+      <c r="F5" s="153"/>
+      <c r="G5" s="153"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="153"/>
+      <c r="J5" s="153"/>
+      <c r="K5" s="153"/>
+      <c r="L5" s="153"/>
+      <c r="M5" s="154"/>
       <c r="N5" s="54"/>
       <c r="O5" s="51"/>
       <c r="P5" s="51"/>
@@ -3693,30 +3693,30 @@
       <c r="AB5" s="59"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="158" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="122"/>
-      <c r="D6" s="121" t="s">
+      <c r="C6" s="159"/>
+      <c r="D6" s="158" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="122"/>
-      <c r="F6" s="121" t="s">
+      <c r="E6" s="159"/>
+      <c r="F6" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="122"/>
-      <c r="H6" s="121" t="s">
+      <c r="G6" s="159"/>
+      <c r="H6" s="158" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="122"/>
-      <c r="J6" s="121" t="s">
+      <c r="I6" s="159"/>
+      <c r="J6" s="158" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="122"/>
-      <c r="L6" s="121" t="s">
+      <c r="K6" s="159"/>
+      <c r="L6" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="M6" s="122"/>
+      <c r="M6" s="159"/>
       <c r="O6" s="59"/>
       <c r="P6" s="59"/>
       <c r="Q6" s="59"/>
@@ -3737,37 +3737,37 @@
         <v>33</v>
       </c>
       <c r="C7" s="49">
-        <v>-20</v>
+        <v>-115</v>
       </c>
       <c r="D7" s="55" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="49">
-        <v>-35</v>
+        <v>-135</v>
       </c>
       <c r="F7" s="55" t="s">
         <v>33</v>
       </c>
       <c r="G7" s="49">
-        <v>-20</v>
+        <v>-115</v>
       </c>
       <c r="H7" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I7" s="49">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="J7" s="55" t="s">
         <v>33</v>
       </c>
       <c r="K7" s="49">
-        <v>35</v>
+        <v>135</v>
       </c>
       <c r="L7" s="55" t="s">
         <v>33</v>
       </c>
       <c r="M7" s="49">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="O7" s="59"/>
       <c r="P7" s="47"/>
@@ -3841,7 +3841,7 @@
         <v>36</v>
       </c>
       <c r="C9" s="50">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="D9" s="56" t="s">
         <v>36</v>
@@ -3853,13 +3853,13 @@
         <v>36</v>
       </c>
       <c r="G9" s="50">
-        <v>-20</v>
+        <v>-70</v>
       </c>
       <c r="H9" s="56" t="s">
         <v>36</v>
       </c>
       <c r="I9" s="50">
-        <v>-20</v>
+        <v>70</v>
       </c>
       <c r="J9" s="56" t="s">
         <v>36</v>
@@ -3871,7 +3871,7 @@
         <v>36</v>
       </c>
       <c r="M9" s="50">
-        <v>20</v>
+        <v>-70</v>
       </c>
       <c r="O9" s="59"/>
       <c r="P9" s="47"/>
@@ -3906,20 +3906,20 @@
       <c r="AB10" s="59"/>
     </row>
     <row r="11" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="155" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="119"/>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
-      <c r="G11" s="119"/>
-      <c r="H11" s="119"/>
-      <c r="I11" s="119"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="119"/>
-      <c r="L11" s="119"/>
-      <c r="M11" s="120"/>
+      <c r="C11" s="156"/>
+      <c r="D11" s="156"/>
+      <c r="E11" s="156"/>
+      <c r="F11" s="156"/>
+      <c r="G11" s="156"/>
+      <c r="H11" s="156"/>
+      <c r="I11" s="156"/>
+      <c r="J11" s="156"/>
+      <c r="K11" s="156"/>
+      <c r="L11" s="156"/>
+      <c r="M11" s="157"/>
       <c r="O11" s="59"/>
       <c r="P11" s="59"/>
       <c r="Q11" s="59"/>
@@ -3936,25 +3936,25 @@
       <c r="AB11" s="59"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B12" s="111" t="s">
+      <c r="B12" s="148" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="112"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="113">
+      <c r="C12" s="149"/>
+      <c r="D12" s="149"/>
+      <c r="E12" s="150">
         <f>TAN((2 - D2) * PI() / 4) * ABS(D3)</f>
-        <v>8.2842712474619002</v>
-      </c>
-      <c r="F12" s="114"/>
-      <c r="G12" s="127" t="s">
+        <v>3.9269916244421305E-2</v>
+      </c>
+      <c r="F12" s="151"/>
+      <c r="G12" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="128"/>
-      <c r="I12" s="128"/>
-      <c r="J12" s="128"/>
-      <c r="K12" s="128"/>
-      <c r="L12" s="128"/>
-      <c r="M12" s="129"/>
+      <c r="H12" s="161"/>
+      <c r="I12" s="161"/>
+      <c r="J12" s="161"/>
+      <c r="K12" s="161"/>
+      <c r="L12" s="161"/>
+      <c r="M12" s="162"/>
       <c r="O12" s="59"/>
       <c r="P12" s="59"/>
       <c r="Q12" s="59"/>
@@ -3971,25 +3971,25 @@
       <c r="AB12" s="59"/>
     </row>
     <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="125" t="s">
+      <c r="B13" s="115" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="126"/>
-      <c r="D13" s="126"/>
-      <c r="E13" s="138">
+      <c r="C13" s="116"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="136">
         <f>SQRT((E12-C7)^2+C9^2)</f>
-        <v>34.641016151377549</v>
-      </c>
-      <c r="F13" s="139"/>
-      <c r="G13" s="135" t="s">
+        <v>134.66266603206154</v>
+      </c>
+      <c r="F13" s="137"/>
+      <c r="G13" s="133" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="136"/>
-      <c r="I13" s="136"/>
-      <c r="J13" s="136"/>
-      <c r="K13" s="136"/>
-      <c r="L13" s="136"/>
-      <c r="M13" s="137"/>
+      <c r="H13" s="134"/>
+      <c r="I13" s="134"/>
+      <c r="J13" s="134"/>
+      <c r="K13" s="134"/>
+      <c r="L13" s="134"/>
+      <c r="M13" s="135"/>
       <c r="O13" s="59"/>
       <c r="P13" s="59"/>
       <c r="Q13" s="59"/>
@@ -4006,23 +4006,23 @@
       <c r="AB13" s="59"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B14" s="125" t="s">
+      <c r="B14" s="115" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="126"/>
-      <c r="D14" s="126"/>
-      <c r="E14" s="138">
+      <c r="C14" s="116"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="136">
         <f>SQRT((E12-E7)^2+E9^2)</f>
-        <v>43.284271247461902</v>
-      </c>
-      <c r="F14" s="139"/>
-      <c r="G14" s="135"/>
-      <c r="H14" s="136"/>
-      <c r="I14" s="136"/>
-      <c r="J14" s="136"/>
-      <c r="K14" s="136"/>
-      <c r="L14" s="136"/>
-      <c r="M14" s="137"/>
+        <v>135.03926991624442</v>
+      </c>
+      <c r="F14" s="137"/>
+      <c r="G14" s="133"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="134"/>
+      <c r="J14" s="134"/>
+      <c r="K14" s="134"/>
+      <c r="L14" s="134"/>
+      <c r="M14" s="135"/>
       <c r="O14" s="59"/>
       <c r="P14" s="59"/>
       <c r="Q14" s="59"/>
@@ -4039,23 +4039,23 @@
       <c r="AB14" s="59"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B15" s="125" t="s">
+      <c r="B15" s="115" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="126"/>
-      <c r="D15" s="126"/>
-      <c r="E15" s="138">
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="136">
         <f>SQRT((E12-G7)^2+G9^2)</f>
-        <v>34.641016151377549</v>
-      </c>
-      <c r="F15" s="139"/>
-      <c r="G15" s="135"/>
-      <c r="H15" s="136"/>
-      <c r="I15" s="136"/>
-      <c r="J15" s="136"/>
-      <c r="K15" s="136"/>
-      <c r="L15" s="136"/>
-      <c r="M15" s="137"/>
+        <v>134.66266603206154</v>
+      </c>
+      <c r="F15" s="137"/>
+      <c r="G15" s="133"/>
+      <c r="H15" s="134"/>
+      <c r="I15" s="134"/>
+      <c r="J15" s="134"/>
+      <c r="K15" s="134"/>
+      <c r="L15" s="134"/>
+      <c r="M15" s="135"/>
       <c r="O15" s="59"/>
       <c r="P15" s="59"/>
       <c r="Q15" s="59"/>
@@ -4072,92 +4072,92 @@
       <c r="AB15" s="59"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B16" s="125" t="s">
+      <c r="B16" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="126"/>
-      <c r="D16" s="126"/>
-      <c r="E16" s="138">
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="136">
         <f>SQRT((E12-I7)^2+I9^2)</f>
-        <v>23.178833020733549</v>
-      </c>
-      <c r="F16" s="139"/>
-      <c r="G16" s="135"/>
-      <c r="H16" s="136"/>
-      <c r="I16" s="136"/>
-      <c r="J16" s="136"/>
-      <c r="K16" s="136"/>
-      <c r="L16" s="136"/>
-      <c r="M16" s="137"/>
+        <v>134.59557742136295</v>
+      </c>
+      <c r="F16" s="137"/>
+      <c r="G16" s="133"/>
+      <c r="H16" s="134"/>
+      <c r="I16" s="134"/>
+      <c r="J16" s="134"/>
+      <c r="K16" s="134"/>
+      <c r="L16" s="134"/>
+      <c r="M16" s="135"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="125" t="s">
+      <c r="B17" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="126"/>
-      <c r="D17" s="126"/>
-      <c r="E17" s="138">
+      <c r="C17" s="116"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="136">
         <f>SQRT((E12-K7)^2+K9^2)</f>
-        <v>26.715728752538098</v>
-      </c>
-      <c r="F17" s="139"/>
-      <c r="G17" s="135"/>
-      <c r="H17" s="136"/>
-      <c r="I17" s="136"/>
-      <c r="J17" s="136"/>
-      <c r="K17" s="136"/>
-      <c r="L17" s="136"/>
-      <c r="M17" s="137"/>
+        <v>134.96073008375558</v>
+      </c>
+      <c r="F17" s="137"/>
+      <c r="G17" s="133"/>
+      <c r="H17" s="134"/>
+      <c r="I17" s="134"/>
+      <c r="J17" s="134"/>
+      <c r="K17" s="134"/>
+      <c r="L17" s="134"/>
+      <c r="M17" s="135"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="125" t="s">
+      <c r="B18" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="126"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="138">
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="136">
         <f>SQRT((E12-M7)^2+M9^2)</f>
-        <v>23.178833020733549</v>
-      </c>
-      <c r="F18" s="139"/>
-      <c r="G18" s="135"/>
-      <c r="H18" s="136"/>
-      <c r="I18" s="136"/>
-      <c r="J18" s="136"/>
-      <c r="K18" s="136"/>
-      <c r="L18" s="136"/>
-      <c r="M18" s="137"/>
+        <v>134.59557742136295</v>
+      </c>
+      <c r="F18" s="137"/>
+      <c r="G18" s="133"/>
+      <c r="H18" s="134"/>
+      <c r="I18" s="134"/>
+      <c r="J18" s="134"/>
+      <c r="K18" s="134"/>
+      <c r="L18" s="134"/>
+      <c r="M18" s="135"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B19" s="125" t="s">
+      <c r="B19" s="115" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="126"/>
-      <c r="D19" s="126"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="116"/>
       <c r="E19" s="48">
         <f>ATAN2(-(E12-C7), C9)</f>
-        <v>2.5261129449194057</v>
+        <v>2.5949554380450901</v>
       </c>
       <c r="F19" s="57">
         <f t="shared" ref="F19:F24" si="0">DEGREES(E19)</f>
-        <v>144.73561031724535</v>
-      </c>
-      <c r="G19" s="142" t="s">
+        <v>148.67999462450544</v>
+      </c>
+      <c r="G19" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="143"/>
-      <c r="I19" s="143"/>
-      <c r="J19" s="143"/>
-      <c r="K19" s="143"/>
-      <c r="L19" s="143"/>
-      <c r="M19" s="144"/>
+      <c r="H19" s="106"/>
+      <c r="I19" s="106"/>
+      <c r="J19" s="106"/>
+      <c r="K19" s="106"/>
+      <c r="L19" s="106"/>
+      <c r="M19" s="107"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="125" t="s">
+      <c r="B20" s="115" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="126"/>
-      <c r="D20" s="126"/>
+      <c r="C20" s="116"/>
+      <c r="D20" s="116"/>
       <c r="E20" s="48">
         <f>ATAN2(-(E12-E7), E9)</f>
         <v>3.1415926535897931</v>
@@ -4166,64 +4166,64 @@
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="G20" s="145"/>
-      <c r="H20" s="146"/>
-      <c r="I20" s="146"/>
-      <c r="J20" s="146"/>
-      <c r="K20" s="146"/>
-      <c r="L20" s="146"/>
-      <c r="M20" s="147"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="109"/>
+      <c r="J20" s="109"/>
+      <c r="K20" s="109"/>
+      <c r="L20" s="109"/>
+      <c r="M20" s="110"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="125" t="s">
+      <c r="B21" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="126"/>
-      <c r="D21" s="126"/>
+      <c r="C21" s="116"/>
+      <c r="D21" s="116"/>
       <c r="E21" s="48">
         <f>ATAN2(-(E12-G7), G9)</f>
-        <v>-2.5261129449194057</v>
+        <v>-2.5949554380450901</v>
       </c>
       <c r="F21" s="57">
         <f t="shared" si="0"/>
-        <v>-144.73561031724535</v>
-      </c>
-      <c r="G21" s="145"/>
-      <c r="H21" s="146"/>
-      <c r="I21" s="146"/>
-      <c r="J21" s="146"/>
-      <c r="K21" s="146"/>
-      <c r="L21" s="146"/>
-      <c r="M21" s="147"/>
+        <v>-148.67999462450544</v>
+      </c>
+      <c r="G21" s="108"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="109"/>
+      <c r="J21" s="109"/>
+      <c r="K21" s="109"/>
+      <c r="L21" s="109"/>
+      <c r="M21" s="110"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="125" t="s">
+      <c r="B22" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="126"/>
-      <c r="D22" s="126"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="116"/>
       <c r="E22" s="48">
         <f>ATAN2(-(E12-I7), I9)</f>
-        <v>-1.04089353704597</v>
+        <v>0.5469405418108203</v>
       </c>
       <c r="F22" s="57">
         <f t="shared" si="0"/>
-        <v>-59.638806595178281</v>
-      </c>
-      <c r="G22" s="145"/>
-      <c r="H22" s="146"/>
-      <c r="I22" s="146"/>
-      <c r="J22" s="146"/>
-      <c r="K22" s="146"/>
-      <c r="L22" s="146"/>
-      <c r="M22" s="147"/>
+        <v>31.337384690358544</v>
+      </c>
+      <c r="G22" s="108"/>
+      <c r="H22" s="109"/>
+      <c r="I22" s="109"/>
+      <c r="J22" s="109"/>
+      <c r="K22" s="109"/>
+      <c r="L22" s="109"/>
+      <c r="M22" s="110"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="125" t="s">
+      <c r="B23" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="126"/>
-      <c r="D23" s="126"/>
+      <c r="C23" s="116"/>
+      <c r="D23" s="116"/>
       <c r="E23" s="48">
         <f>ATAN2(-(E12-K7), K9)</f>
         <v>0</v>
@@ -4232,139 +4232,139 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="145"/>
-      <c r="H23" s="146"/>
-      <c r="I23" s="146"/>
-      <c r="J23" s="146"/>
-      <c r="K23" s="146"/>
-      <c r="L23" s="146"/>
-      <c r="M23" s="147"/>
+      <c r="G23" s="108"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="109"/>
+      <c r="J23" s="109"/>
+      <c r="K23" s="109"/>
+      <c r="L23" s="109"/>
+      <c r="M23" s="110"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="125" t="s">
+      <c r="B24" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="126"/>
-      <c r="D24" s="126"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
       <c r="E24" s="48">
         <f>ATAN2(-(E12-M7), M9)</f>
-        <v>1.04089353704597</v>
+        <v>-0.5469405418108203</v>
       </c>
       <c r="F24" s="57">
         <f t="shared" si="0"/>
-        <v>59.638806595178281</v>
-      </c>
-      <c r="G24" s="148"/>
-      <c r="H24" s="149"/>
-      <c r="I24" s="149"/>
-      <c r="J24" s="149"/>
-      <c r="K24" s="149"/>
-      <c r="L24" s="149"/>
-      <c r="M24" s="150"/>
+        <v>-31.337384690358544</v>
+      </c>
+      <c r="G24" s="111"/>
+      <c r="H24" s="112"/>
+      <c r="I24" s="112"/>
+      <c r="J24" s="112"/>
+      <c r="K24" s="112"/>
+      <c r="L24" s="112"/>
+      <c r="M24" s="113"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="123" t="s">
+      <c r="B25" s="138" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="124"/>
-      <c r="D25" s="124"/>
-      <c r="E25" s="158">
+      <c r="C25" s="139"/>
+      <c r="D25" s="139"/>
+      <c r="E25" s="123">
         <f>MAX(E13:F18)</f>
-        <v>43.284271247461902</v>
-      </c>
-      <c r="F25" s="159"/>
-      <c r="G25" s="160"/>
-      <c r="H25" s="161"/>
-      <c r="I25" s="161"/>
-      <c r="J25" s="161"/>
-      <c r="K25" s="161"/>
-      <c r="L25" s="161"/>
-      <c r="M25" s="162"/>
+        <v>135.03926991624442</v>
+      </c>
+      <c r="F25" s="124"/>
+      <c r="G25" s="125"/>
+      <c r="H25" s="126"/>
+      <c r="I25" s="126"/>
+      <c r="J25" s="126"/>
+      <c r="K25" s="126"/>
+      <c r="L25" s="126"/>
+      <c r="M25" s="127"/>
     </row>
     <row r="26" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="130" t="s">
+      <c r="B26" s="128" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="131"/>
-      <c r="D26" s="131"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129"/>
       <c r="E26" s="74">
         <f>SIGN(E12) * D3 / E25</f>
-        <v>-0.46206160860737044</v>
+        <v>0.37026266530477814</v>
       </c>
       <c r="F26" s="75">
         <f>ABS(E26)</f>
-        <v>0.46206160860737044</v>
-      </c>
-      <c r="G26" s="132" t="s">
+        <v>0.37026266530477814</v>
+      </c>
+      <c r="G26" s="130" t="s">
         <v>47</v>
       </c>
-      <c r="H26" s="133"/>
-      <c r="I26" s="133"/>
-      <c r="J26" s="133"/>
-      <c r="K26" s="133"/>
-      <c r="L26" s="133"/>
-      <c r="M26" s="134"/>
+      <c r="H26" s="131"/>
+      <c r="I26" s="131"/>
+      <c r="J26" s="131"/>
+      <c r="K26" s="131"/>
+      <c r="L26" s="131"/>
+      <c r="M26" s="132"/>
     </row>
     <row r="29" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="151" t="s">
+      <c r="B29" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="151"/>
-      <c r="D29" s="151"/>
-      <c r="E29" s="151"/>
-      <c r="F29" s="151"/>
-      <c r="G29" s="151"/>
-      <c r="H29" s="151"/>
-      <c r="I29" s="151"/>
-      <c r="J29" s="151"/>
-      <c r="K29" s="151"/>
-      <c r="L29" s="151"/>
-      <c r="M29" s="151"/>
-      <c r="N29" s="151"/>
-      <c r="O29" s="151"/>
-      <c r="P29" s="151"/>
-      <c r="Q29" s="151"/>
-      <c r="R29" s="151"/>
-      <c r="S29" s="151"/>
-      <c r="T29" s="151"/>
+      <c r="C29" s="114"/>
+      <c r="D29" s="114"/>
+      <c r="E29" s="114"/>
+      <c r="F29" s="114"/>
+      <c r="G29" s="114"/>
+      <c r="H29" s="114"/>
+      <c r="I29" s="114"/>
+      <c r="J29" s="114"/>
+      <c r="K29" s="114"/>
+      <c r="L29" s="114"/>
+      <c r="M29" s="114"/>
+      <c r="N29" s="114"/>
+      <c r="O29" s="114"/>
+      <c r="P29" s="114"/>
+      <c r="Q29" s="114"/>
+      <c r="R29" s="114"/>
+      <c r="S29" s="114"/>
+      <c r="T29" s="114"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="140" t="s">
+      <c r="B30" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="155" t="s">
+      <c r="C30" s="120" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="156"/>
-      <c r="E30" s="157"/>
-      <c r="F30" s="152" t="s">
+      <c r="D30" s="121"/>
+      <c r="E30" s="122"/>
+      <c r="F30" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="153"/>
-      <c r="H30" s="154"/>
-      <c r="I30" s="155" t="s">
+      <c r="G30" s="118"/>
+      <c r="H30" s="119"/>
+      <c r="I30" s="120" t="s">
         <v>50</v>
       </c>
-      <c r="J30" s="156"/>
-      <c r="K30" s="157"/>
-      <c r="L30" s="152" t="s">
+      <c r="J30" s="121"/>
+      <c r="K30" s="122"/>
+      <c r="L30" s="117" t="s">
         <v>51</v>
       </c>
-      <c r="M30" s="153"/>
-      <c r="N30" s="154"/>
-      <c r="O30" s="155" t="s">
+      <c r="M30" s="118"/>
+      <c r="N30" s="119"/>
+      <c r="O30" s="120" t="s">
         <v>52</v>
       </c>
-      <c r="P30" s="156"/>
-      <c r="Q30" s="157"/>
-      <c r="R30" s="152" t="s">
+      <c r="P30" s="121"/>
+      <c r="Q30" s="122"/>
+      <c r="R30" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="S30" s="153"/>
-      <c r="T30" s="154"/>
+      <c r="S30" s="118"/>
+      <c r="T30" s="119"/>
     </row>
     <row r="31" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="141"/>
+      <c r="B31" s="104"/>
       <c r="C31" s="62" t="s">
         <v>60</v>
       </c>
@@ -4426,75 +4426,75 @@
       </c>
       <c r="C32" s="81">
         <f>($B32-0.5) * $E$26 + $E$19</f>
-        <v>2.7571437492230908</v>
+        <v>2.4098241053927012</v>
       </c>
       <c r="D32" s="82">
         <f>$E$12+$E$13*COS(C32)</f>
-        <v>-23.82813296867765</v>
+        <v>-100.14892496555947</v>
       </c>
       <c r="E32" s="83">
         <f>$E$13*SIN(C32)</f>
-        <v>12.992055089910252</v>
+        <v>89.979771222137614</v>
       </c>
       <c r="F32" s="84">
         <f>($B32 - 0.5) * $E$26 + $E$20</f>
-        <v>3.3726234578934782</v>
+        <v>2.9564613209374042</v>
       </c>
       <c r="G32" s="85">
         <f>$E$12+$E$14*COS(F32)</f>
-        <v>-33.849974896909735</v>
+        <v>-132.69246029453819</v>
       </c>
       <c r="H32" s="86">
         <f>$E$14*SIN(F32)</f>
-        <v>-9.9112783872395216</v>
+        <v>24.857437815759159</v>
       </c>
       <c r="I32" s="81">
         <f>($B32 - 0.5) * $E$26 + $E$21</f>
-        <v>-2.2950821406157207</v>
+        <v>-2.780086770697479</v>
       </c>
       <c r="J32" s="82">
         <f>$E$12+$E$15*COS(I32)</f>
-        <v>-14.668890498750928</v>
+        <v>-125.91951226482961</v>
       </c>
       <c r="K32" s="83">
         <f>$E$15*SIN(I32)</f>
-        <v>-25.945180011944267</v>
+        <v>-47.62792053326794</v>
       </c>
       <c r="L32" s="84">
         <f xml:space="preserve"> ($B32 - 0.5) * $E$26 + $E$22</f>
-        <v>-0.80986273274228471</v>
+        <v>0.36180920915843123</v>
       </c>
       <c r="M32" s="85">
         <f>$E$12+$E$16*COS(L32)</f>
-        <v>24.268344603103579</v>
+        <v>125.92085434689243</v>
       </c>
       <c r="N32" s="86">
         <f>$E$16*SIN(L32)</f>
-        <v>-16.785937542017532</v>
+        <v>47.642377801908076</v>
       </c>
       <c r="O32" s="81">
         <f>($B32 - 0.5) * $E$26 + $E$23</f>
-        <v>0.23103080430368522</v>
+        <v>-0.18513133265238907</v>
       </c>
       <c r="P32" s="82">
         <f>$E$12+$E$17*COS(O32)</f>
-        <v>34.29018653133565</v>
+        <v>132.69380237660101</v>
       </c>
       <c r="Q32" s="83">
         <f>$E$17*SIN(O32)</f>
-        <v>6.1173959351322393</v>
+        <v>-24.842980547118994</v>
       </c>
       <c r="R32" s="84">
         <f>($B32 - 0.5) * $E$26 + $E$24</f>
-        <v>1.2719243413496553</v>
+        <v>-0.73207187446320932</v>
       </c>
       <c r="S32" s="85">
         <f>$E$12+$E$18*COS(R32)</f>
-        <v>15.109102133176851</v>
+        <v>100.15026704762228</v>
       </c>
       <c r="T32" s="86">
         <f>$E$18*SIN(R32)</f>
-        <v>22.151297559836966</v>
+        <v>-89.965313953497443</v>
       </c>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
@@ -4503,75 +4503,75 @@
       </c>
       <c r="C33" s="65">
         <f t="shared" ref="C33:C52" si="1">($B33-0.5) * $E$26 + $E$19</f>
-        <v>2.7340406687927223</v>
+        <v>2.42833723865794</v>
       </c>
       <c r="D33" s="66">
         <f t="shared" ref="D33:D52" si="2">$E$12+$E$13*COS(C33)</f>
-        <v>-23.519433521775909</v>
+        <v>-101.79746874221689</v>
       </c>
       <c r="E33" s="67">
         <f t="shared" ref="E33:E52" si="3">$E$13*SIN(C33)</f>
-        <v>13.730417435430004</v>
+        <v>88.109660550196153</v>
       </c>
       <c r="F33" s="71">
         <f t="shared" ref="F33:F52" si="4">($B33 - 0.5) * $E$26 + $E$20</f>
-        <v>3.3495203774631097</v>
+        <v>2.9749744542026431</v>
       </c>
       <c r="G33" s="72">
         <f t="shared" ref="G33:G52" si="5">$E$12+$E$14*COS(F33)</f>
-        <v>-34.067691463555342</v>
+        <v>-133.12987773832018</v>
       </c>
       <c r="H33" s="73">
         <f t="shared" ref="H33:H52" si="6">$E$14*SIN(F33)</f>
-        <v>-8.9352891362541698</v>
+        <v>22.396038320852366</v>
       </c>
       <c r="I33" s="65">
         <f t="shared" ref="I33:I52" si="7">($B33 - 0.5) * $E$26 + $E$21</f>
-        <v>-2.3181852210460892</v>
+        <v>-2.7615736374322402</v>
       </c>
       <c r="J33" s="66">
         <f t="shared" ref="J33:J52" si="8">$E$12+$E$15*COS(I33)</f>
-        <v>-15.262125378436776</v>
+        <v>-125.01623589686776</v>
       </c>
       <c r="K33" s="67">
         <f t="shared" ref="K33:K52" si="9">$E$15*SIN(I33)</f>
-        <v>-25.408014600434004</v>
+        <v>-49.951517381248848</v>
       </c>
       <c r="L33" s="71">
         <f t="shared" ref="L33:L52" si="10" xml:space="preserve"> ($B33 - 0.5) * $E$26 + $E$22</f>
-        <v>-0.83296581317265328</v>
+        <v>0.38032234242367013</v>
       </c>
       <c r="M33" s="72">
         <f t="shared" ref="M33:M52" si="11">$E$12+$E$16*COS(L33)</f>
-        <v>23.876306657427222</v>
+        <v>125.01732357372842</v>
       </c>
       <c r="N33" s="73">
         <f t="shared" ref="N33:N52" si="12">$E$16*SIN(L33)</f>
-        <v>-17.150706457094863</v>
+        <v>49.964543081841143</v>
       </c>
       <c r="O33" s="65">
         <f t="shared" ref="O33:O52" si="13">($B33 - 0.5) * $E$26 + $E$23</f>
-        <v>0.20792772387331671</v>
+        <v>-0.16661819938715017</v>
       </c>
       <c r="P33" s="66">
         <f t="shared" ref="P33:P52" si="14">$E$12+$E$17*COS(O33)</f>
-        <v>34.424564599206647</v>
+        <v>133.13096541518081</v>
       </c>
       <c r="Q33" s="67">
         <f t="shared" ref="Q33:Q52" si="15">$E$17*SIN(O33)</f>
-        <v>5.5150001145893084</v>
+        <v>-22.383012620260054</v>
       </c>
       <c r="R33" s="71">
         <f t="shared" ref="R33:R52" si="16">($B33 - 0.5) * $E$26 + $E$24</f>
-        <v>1.2488212609192866</v>
+        <v>-0.71355874119797047</v>
       </c>
       <c r="S33" s="72">
         <f t="shared" ref="S33:S52" si="17">$E$12+$E$18*COS(R33)</f>
-        <v>15.618998514088089</v>
+        <v>101.79855641907753</v>
       </c>
       <c r="T33" s="73">
         <f t="shared" ref="T33:T52" si="18">$E$18*SIN(R33)</f>
-        <v>21.98772557876913</v>
+        <v>-88.096634849603845</v>
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
@@ -4580,75 +4580,75 @@
       </c>
       <c r="C34" s="65">
         <f t="shared" si="1"/>
-        <v>2.7109375883623539</v>
+        <v>2.4468503719231789</v>
       </c>
       <c r="D34" s="66">
         <f t="shared" si="2"/>
-        <v>-23.19375952853526</v>
+        <v>-103.41111038876282</v>
       </c>
       <c r="E34" s="67">
         <f t="shared" si="3"/>
-        <v>14.461451464682787</v>
+        <v>86.209352379030832</v>
       </c>
       <c r="F34" s="71">
         <f t="shared" si="4"/>
-        <v>3.3264172970327412</v>
+        <v>2.9934875874678819</v>
       </c>
       <c r="G34" s="72">
         <f t="shared" si="5"/>
-        <v>-34.26280357707833</v>
+        <v>-133.52165461093401</v>
       </c>
       <c r="H34" s="73">
         <f t="shared" si="6"/>
-        <v>-7.9545308660430551</v>
+        <v>19.926963114274585</v>
       </c>
       <c r="I34" s="65">
         <f t="shared" si="7"/>
-        <v>-2.3412883014764576</v>
+        <v>-2.7430605041670013</v>
       </c>
       <c r="J34" s="66">
         <f t="shared" si="8"/>
-        <v>-15.842792873173584</v>
+        <v>-124.07009971630248</v>
       </c>
       <c r="K34" s="67">
         <f t="shared" si="9"/>
-        <v>-24.857288205247652</v>
+        <v>-52.257994529778742</v>
       </c>
       <c r="L34" s="71">
         <f t="shared" si="10"/>
-        <v>-0.85606889360302185</v>
+        <v>0.39883547568890904</v>
       </c>
       <c r="M34" s="72">
         <f t="shared" si="11"/>
-        <v>23.475946796756844</v>
+        <v>124.07095953285281</v>
       </c>
       <c r="N34" s="73">
         <f t="shared" si="12"/>
-        <v>-17.506321549885975</v>
+        <v>52.26958419807282</v>
       </c>
       <c r="O34" s="65">
         <f t="shared" si="13"/>
-        <v>0.18482464344294819</v>
+        <v>-0.14810506612191127</v>
       </c>
       <c r="P34" s="66">
         <f t="shared" si="14"/>
-        <v>34.544990845299921</v>
+        <v>133.52251442748434</v>
       </c>
       <c r="Q34" s="67">
         <f t="shared" si="15"/>
-        <v>4.909660780839868</v>
+        <v>-19.915373445980478</v>
       </c>
       <c r="R34" s="71">
         <f t="shared" si="16"/>
-        <v>1.2257181804889181</v>
+        <v>-0.69504560793273162</v>
       </c>
       <c r="S34" s="72">
         <f t="shared" si="17"/>
-        <v>16.124980141395174</v>
+        <v>103.41197020531315</v>
       </c>
       <c r="T34" s="73">
         <f t="shared" si="18"/>
-        <v>21.812418120044455</v>
+        <v>-86.197762710736725</v>
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
@@ -4657,75 +4657,75 @@
       </c>
       <c r="C35" s="65">
         <f t="shared" si="1"/>
-        <v>2.6878345079319854</v>
+        <v>2.4653635051884177</v>
       </c>
       <c r="D35" s="66">
         <f t="shared" si="2"/>
-        <v>-22.851284810475221</v>
+        <v>-104.98929686774301</v>
       </c>
       <c r="E35" s="67">
         <f t="shared" si="3"/>
-        <v>15.184767003910704</v>
+        <v>84.279497994257369</v>
       </c>
       <c r="F35" s="71">
         <f t="shared" si="4"/>
-        <v>3.3033142166023728</v>
+        <v>3.0120007207331208</v>
       </c>
       <c r="G35" s="72">
         <f t="shared" si="5"/>
-        <v>-34.435207100566458</v>
+        <v>-133.86765664013609</v>
       </c>
       <c r="H35" s="73">
         <f t="shared" si="6"/>
-        <v>-6.9695270353298016</v>
+        <v>17.451058413071362</v>
       </c>
       <c r="I35" s="65">
         <f t="shared" si="7"/>
-        <v>-2.3643913819068261</v>
+        <v>-2.7245473709017625</v>
       </c>
       <c r="J35" s="66">
         <f t="shared" si="8"/>
-        <v>-16.410583064121127</v>
+        <v>-123.08142798889988</v>
       </c>
       <c r="K35" s="67">
         <f t="shared" si="9"/>
-        <v>-24.293294764804742</v>
+        <v>-54.546561488445221</v>
       </c>
       <c r="L35" s="71">
         <f t="shared" si="10"/>
-        <v>-0.87917197403339031</v>
+        <v>0.41734860895414794</v>
       </c>
       <c r="M35" s="72">
         <f t="shared" si="11"/>
-        <v>23.067478704594315</v>
+        <v>123.08208656812548</v>
       </c>
       <c r="N35" s="73">
         <f t="shared" si="12"/>
-        <v>-17.852593018450641</v>
+        <v>54.556711152356797</v>
       </c>
       <c r="O35" s="65">
         <f t="shared" si="13"/>
-        <v>0.16172156301257964</v>
+        <v>-0.12959193285667234</v>
       </c>
       <c r="P35" s="66">
         <f t="shared" si="14"/>
-        <v>34.651400994685552</v>
+        <v>133.86831521936168</v>
       </c>
       <c r="Q35" s="67">
         <f t="shared" si="15"/>
-        <v>4.3017010207898609</v>
+        <v>-17.440908749159757</v>
       </c>
       <c r="R35" s="71">
         <f t="shared" si="16"/>
-        <v>1.2026151000585497</v>
+        <v>-0.67653247466749267</v>
       </c>
       <c r="S35" s="72">
         <f t="shared" si="17"/>
-        <v>16.626776958240217</v>
+        <v>104.98995544696859</v>
       </c>
       <c r="T35" s="73">
         <f t="shared" si="18"/>
-        <v>21.625468750264794</v>
+        <v>-84.269348330345778</v>
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
@@ -4734,75 +4734,75 @@
       </c>
       <c r="C36" s="65">
         <f t="shared" si="1"/>
-        <v>2.664731427501617</v>
+        <v>2.4838766384536566</v>
       </c>
       <c r="D36" s="66">
         <f t="shared" si="2"/>
-        <v>-22.492192156142416</v>
+        <v>-106.53148729312204</v>
       </c>
       <c r="E36" s="67">
         <f t="shared" si="3"/>
-        <v>15.899977998934611</v>
+        <v>82.32075880775642</v>
       </c>
       <c r="F36" s="71">
         <f t="shared" si="4"/>
-        <v>3.2802111361720043</v>
+        <v>3.0305138539983596</v>
       </c>
       <c r="G36" s="72">
         <f t="shared" si="5"/>
-        <v>-34.584810017331122</v>
+        <v>-134.16776524192616</v>
       </c>
       <c r="H36" s="73">
         <f t="shared" si="6"/>
-        <v>-5.9808033688150299</v>
+        <v>14.969172774935751</v>
       </c>
       <c r="I36" s="65">
         <f t="shared" si="7"/>
-        <v>-2.3874944623371945</v>
+        <v>-2.7060342376365236</v>
       </c>
       <c r="J36" s="66">
         <f t="shared" si="8"/>
-        <v>-16.965192905424296</v>
+        <v>-122.05055955847723</v>
       </c>
       <c r="K36" s="67">
         <f t="shared" si="9"/>
-        <v>-23.716335298526101</v>
+        <v>-56.816433905129294</v>
       </c>
       <c r="L36" s="71">
         <f t="shared" si="10"/>
-        <v>-0.90227505446375889</v>
+        <v>0.43586174221938689</v>
       </c>
       <c r="M36" s="72">
         <f t="shared" si="11"/>
-        <v>22.6511203920364</v>
+        <v>122.05104359233296</v>
       </c>
       <c r="N36" s="73">
         <f t="shared" si="12"/>
-        <v>-18.189336047807984</v>
+        <v>56.825140086101463</v>
       </c>
       <c r="O36" s="65">
         <f t="shared" si="13"/>
-        <v>0.13861848258221113</v>
+        <v>-0.11107879959143344</v>
       </c>
       <c r="P36" s="66">
         <f t="shared" si="14"/>
-        <v>34.743738253225104</v>
+        <v>134.1682492757819</v>
       </c>
       <c r="Q36" s="67">
         <f t="shared" si="15"/>
-        <v>3.6914453199416575</v>
+        <v>-14.960466593963559</v>
       </c>
       <c r="R36" s="71">
         <f t="shared" si="16"/>
-        <v>1.1795120196281812</v>
+        <v>-0.65801934140225371</v>
       </c>
       <c r="S36" s="72">
         <f t="shared" si="17"/>
-        <v>17.124121141318291</v>
+        <v>106.53197132697777</v>
       </c>
       <c r="T36" s="73">
         <f t="shared" si="18"/>
-        <v>21.426977249652715</v>
+        <v>-82.312052626784237</v>
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
@@ -4811,75 +4811,75 @@
       </c>
       <c r="C37" s="65">
         <f t="shared" si="1"/>
-        <v>2.6416283470712485</v>
+        <v>2.5023897717188954</v>
       </c>
       <c r="D37" s="66">
         <f t="shared" si="2"/>
-        <v>-22.116673223551054</v>
+        <v>-108.03715311565934</v>
       </c>
       <c r="E37" s="67">
         <f t="shared" si="3"/>
-        <v>16.606702721202282</v>
+        <v>80.33380613099024</v>
       </c>
       <c r="F37" s="71">
         <f t="shared" si="4"/>
-        <v>3.2571080557416359</v>
+        <v>3.0490269872635984</v>
       </c>
       <c r="G37" s="72">
         <f t="shared" si="5"/>
-        <v>-34.711532480019251</v>
+        <v>-134.42187756118923</v>
       </c>
       <c r="H37" s="73">
         <f t="shared" si="6"/>
-        <v>-4.9888875765820613</v>
+        <v>12.482156807385293</v>
       </c>
       <c r="I37" s="65">
         <f t="shared" si="7"/>
-        <v>-2.410597542767563</v>
+        <v>-2.6875211043712848</v>
       </c>
       <c r="J37" s="66">
         <f t="shared" si="8"/>
-        <v>-17.506326385957379</v>
+        <v>-120.97784773077237</v>
       </c>
       <c r="K37" s="67">
         <f t="shared" si="9"/>
-        <v>-23.126717746171163</v>
+        <v>-59.066833834823406</v>
       </c>
       <c r="L37" s="71">
         <f t="shared" si="10"/>
-        <v>-0.92537813489412735</v>
+        <v>0.45437487548462574</v>
       </c>
       <c r="M37" s="72">
         <f t="shared" si="11"/>
-        <v>22.227094081416055</v>
+        <v>120.9781839710344</v>
       </c>
       <c r="N37" s="73">
         <f t="shared" si="12"/>
-        <v>-18.516370908577485</v>
+        <v>59.074093549018841</v>
       </c>
       <c r="O37" s="65">
         <f t="shared" si="13"/>
-        <v>0.11551540215184261</v>
+        <v>-9.2565666326194534E-2</v>
       </c>
       <c r="P37" s="66">
         <f t="shared" si="14"/>
-        <v>34.821953337884253</v>
+        <v>134.42221380145125</v>
       </c>
       <c r="Q37" s="67">
         <f t="shared" si="15"/>
-        <v>3.0792193892068549</v>
+        <v>-12.474897093189828</v>
       </c>
       <c r="R37" s="71">
         <f t="shared" si="16"/>
-        <v>1.1564089391978125</v>
+        <v>-0.63950620813701486</v>
       </c>
       <c r="S37" s="72">
         <f t="shared" si="17"/>
-        <v>17.616747243822388</v>
+        <v>108.03748935592138</v>
       </c>
       <c r="T37" s="73">
         <f t="shared" si="18"/>
-        <v>21.217049558795946</v>
+        <v>-80.326546416794784</v>
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
@@ -4888,75 +4888,75 @@
       </c>
       <c r="C38" s="65">
         <f t="shared" si="1"/>
-        <v>2.61852526664088</v>
+        <v>2.5209029049841343</v>
       </c>
       <c r="D38" s="66">
         <f t="shared" si="2"/>
-        <v>-21.724928437889609</v>
+        <v>-109.50577830405679</v>
       </c>
       <c r="E38" s="67">
         <f t="shared" si="3"/>
-        <v>17.304563971527834</v>
+        <v>78.319320944926616</v>
       </c>
       <c r="F38" s="71">
         <f t="shared" si="4"/>
-        <v>3.2340049753112674</v>
+        <v>3.0675401205288373</v>
       </c>
       <c r="G38" s="72">
         <f t="shared" si="5"/>
-        <v>-34.81530685323019</v>
+        <v>-134.62990650694664</v>
       </c>
       <c r="H38" s="73">
         <f t="shared" si="6"/>
-        <v>-3.9943090724429551</v>
+        <v>9.9908628762364113</v>
       </c>
       <c r="I38" s="65">
         <f t="shared" si="7"/>
-        <v>-2.4337006231979315</v>
+        <v>-2.6690079711060459</v>
       </c>
       <c r="J38" s="66">
         <f t="shared" si="8"/>
-        <v>-18.033694687313591</v>
+        <v>-119.86366015235637</v>
       </c>
       <c r="K38" s="67">
         <f t="shared" si="9"/>
-        <v>-22.524756803481743</v>
+        <v>-61.296990006253715</v>
       </c>
       <c r="L38" s="71">
         <f t="shared" si="10"/>
-        <v>-0.94848121532449592</v>
+        <v>0.4728880087498647</v>
       </c>
       <c r="M38" s="72">
         <f t="shared" si="11"/>
-        <v>21.795626087695972</v>
+        <v>119.86387540145367</v>
       </c>
       <c r="N38" s="73">
         <f t="shared" si="12"/>
-        <v>-18.833523052905722</v>
+        <v>61.302800765577338</v>
       </c>
       <c r="O38" s="65">
         <f t="shared" si="13"/>
-        <v>9.2412321721474094E-2</v>
+        <v>-7.4052533060955633E-2</v>
       </c>
       <c r="P38" s="66">
         <f t="shared" si="14"/>
-        <v>34.886004503036553</v>
+        <v>134.63012175604393</v>
       </c>
       <c r="Q38" s="67">
         <f t="shared" si="15"/>
-        <v>2.4653499910650627</v>
+        <v>-9.9850521169127635</v>
       </c>
       <c r="R38" s="71">
         <f t="shared" si="16"/>
-        <v>1.1333058587674441</v>
+        <v>-0.62099307487177591</v>
       </c>
       <c r="S38" s="72">
         <f t="shared" si="17"/>
-        <v>18.104392337119965</v>
+        <v>109.50599355315411</v>
       </c>
       <c r="T38" s="73">
         <f t="shared" si="18"/>
-        <v>20.995797722103841</v>
+        <v>-78.313510185602979</v>
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
@@ -4965,75 +4965,75 @@
       </c>
       <c r="C39" s="65">
         <f t="shared" si="1"/>
-        <v>2.5954221862105111</v>
+        <v>2.5394160382493736</v>
       </c>
       <c r="D39" s="66">
         <f t="shared" si="2"/>
-        <v>-21.317166884548143</v>
+        <v>-110.93685952181639</v>
       </c>
       <c r="E39" s="67">
         <f t="shared" si="3"/>
-        <v>17.993189281413734</v>
+        <v>76.277993666648783</v>
       </c>
       <c r="F39" s="71">
         <f t="shared" si="4"/>
-        <v>3.2109018948808985</v>
+        <v>3.0860532537940766</v>
       </c>
       <c r="G39" s="72">
         <f t="shared" si="5"/>
-        <v>-34.896077749614562</v>
+        <v>-134.79178078220454</v>
       </c>
       <c r="H39" s="73">
         <f t="shared" si="6"/>
-        <v>-2.9975986913752113</v>
+        <v>7.4961448134761683</v>
       </c>
       <c r="I39" s="65">
         <f t="shared" si="7"/>
-        <v>-2.4568037036283004</v>
+        <v>-2.6504948378408066</v>
       </c>
       <c r="J39" s="66">
         <f t="shared" si="8"/>
-        <v>-18.547016337955782</v>
+        <v>-118.70837868463155</v>
       </c>
       <c r="K39" s="67">
         <f t="shared" si="9"/>
-        <v>-21.910773754219893</v>
+        <v>-63.506138086215103</v>
       </c>
       <c r="L39" s="71">
         <f t="shared" si="10"/>
-        <v>-0.97158429575486438</v>
+        <v>0.49140114201510354</v>
       </c>
       <c r="M39" s="72">
         <f t="shared" si="11"/>
-        <v>21.356946697677845</v>
+        <v>118.70849978645992</v>
       </c>
       <c r="N39" s="73">
         <f t="shared" si="12"/>
-        <v>-19.140623207627524</v>
+        <v>63.510497899166715</v>
       </c>
       <c r="O39" s="65">
         <f t="shared" si="13"/>
-        <v>6.9309241291105578E-2</v>
+        <v>-5.5539399795716732E-2</v>
       </c>
       <c r="P39" s="66">
         <f t="shared" si="14"/>
-        <v>34.93585756274426</v>
+        <v>134.79190188403288</v>
       </c>
       <c r="Q39" s="67">
         <f t="shared" si="15"/>
-        <v>1.8501647651614226</v>
+        <v>-7.4917850005245246</v>
       </c>
       <c r="R39" s="71">
         <f t="shared" si="16"/>
-        <v>1.1102027783370756</v>
+        <v>-0.60247994160653706</v>
       </c>
       <c r="S39" s="72">
         <f t="shared" si="17"/>
-        <v>18.586796151085473</v>
+        <v>110.93698062364474</v>
       </c>
       <c r="T39" s="73">
         <f t="shared" si="18"/>
-        <v>20.763339828006092</v>
+        <v>-76.273633853697149</v>
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
@@ -5042,75 +5042,75 @@
       </c>
       <c r="C40" s="65">
         <f t="shared" si="1"/>
-        <v>2.5723191057801427</v>
+        <v>2.5579291715146124</v>
       </c>
       <c r="D40" s="66">
         <f t="shared" si="2"/>
-        <v>-20.893606197523482</v>
+        <v>-112.32990629974668</v>
       </c>
       <c r="E40" s="67">
         <f t="shared" si="3"/>
-        <v>18.67221111184783</v>
+        <v>74.210523912731404</v>
       </c>
       <c r="F40" s="71">
         <f t="shared" si="4"/>
-        <v>3.18779881445053</v>
+        <v>3.1045663870593154</v>
       </c>
       <c r="G40" s="72">
         <f t="shared" si="5"/>
-        <v>-34.953802059436164</v>
+        <v>-134.90744490838915</v>
       </c>
       <c r="H40" s="73">
         <f t="shared" si="6"/>
-        <v>-1.9992884062000433</v>
+        <v>4.9988576246318139</v>
       </c>
       <c r="I40" s="65">
         <f t="shared" si="7"/>
-        <v>-2.4799067840586688</v>
+        <v>-2.6319817045755678</v>
       </c>
       <c r="J40" s="66">
         <f t="shared" si="8"/>
-        <v>-19.046017363445763</v>
+        <v>-117.51239927295748</v>
       </c>
       <c r="K40" s="67">
         <f t="shared" si="9"/>
-        <v>-21.285096298689638</v>
+        <v>-65.693520941528021</v>
       </c>
       <c r="L40" s="71">
         <f t="shared" si="10"/>
-        <v>-0.99468737618523295</v>
+        <v>0.5099142752803425</v>
       </c>
       <c r="M40" s="72">
         <f t="shared" si="11"/>
-        <v>20.911290047091697</v>
+        <v>117.51245310367943</v>
       </c>
       <c r="N40" s="73">
         <f t="shared" si="12"/>
-        <v>-19.437507464611908</v>
+        <v>65.696428313885079</v>
       </c>
       <c r="O40" s="65">
         <f t="shared" si="13"/>
-        <v>4.6206160860737033E-2</v>
+        <v>-3.7026266530477803E-2</v>
       </c>
       <c r="P40" s="66">
         <f t="shared" si="14"/>
-        <v>34.971485909004379</v>
+        <v>134.90749873911111</v>
       </c>
       <c r="Q40" s="67">
         <f t="shared" si="15"/>
-        <v>1.2339920534359656</v>
+        <v>-4.9959502522747368</v>
       </c>
       <c r="R40" s="71">
         <f t="shared" si="16"/>
-        <v>1.0870996979067069</v>
+        <v>-0.5839668083412981</v>
       </c>
       <c r="S40" s="72">
         <f t="shared" si="17"/>
-        <v>19.063701213013974</v>
+        <v>112.32996013046863</v>
       </c>
       <c r="T40" s="73">
         <f t="shared" si="18"/>
-        <v>20.519799945925545</v>
+        <v>-74.207616540374318</v>
       </c>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
@@ -5119,75 +5119,75 @@
       </c>
       <c r="C41" s="65">
         <f t="shared" si="1"/>
-        <v>2.5492160253497742</v>
+        <v>2.5764423047798513</v>
       </c>
       <c r="D41" s="66">
         <f t="shared" si="2"/>
-        <v>-20.454472443261693</v>
+        <v>-113.68444120405972</v>
       </c>
       <c r="E41" s="67">
         <f t="shared" si="3"/>
-        <v>19.341267049469508</v>
+        <v>72.117620259463308</v>
       </c>
       <c r="F41" s="71">
         <f t="shared" si="4"/>
-        <v>3.1646957340201616</v>
+        <v>3.1230795203245543</v>
       </c>
       <c r="G41" s="72">
         <f t="shared" si="5"/>
-        <v>-34.988448973580795</v>
+        <v>-134.97685924436081</v>
       </c>
       <c r="H41" s="73">
         <f t="shared" si="6"/>
-        <v>-0.99991104365316275</v>
+        <v>2.4998571957375324</v>
       </c>
       <c r="I41" s="65">
         <f t="shared" si="7"/>
-        <v>-2.5030098644890373</v>
+        <v>-2.6134685713103289</v>
       </c>
       <c r="J41" s="66">
         <f t="shared" si="8"/>
-        <v>-19.53043143267238</v>
+        <v>-116.27613181094999</v>
       </c>
       <c r="K41" s="67">
         <f t="shared" si="9"/>
-        <v>-20.648058378833856</v>
+        <v>-67.858388898528361</v>
       </c>
       <c r="L41" s="71">
         <f t="shared" si="10"/>
-        <v>-1.0177904566156015</v>
+        <v>0.52842740854558135</v>
       </c>
       <c r="M41" s="72">
         <f t="shared" si="11"/>
-        <v>20.458893995630973</v>
+        <v>116.27614526978367</v>
       </c>
       <c r="N41" s="73">
         <f t="shared" si="12"/>
-        <v>-19.724017368244535</v>
+        <v>67.859842833857826</v>
       </c>
       <c r="O41" s="65">
         <f t="shared" si="13"/>
-        <v>2.3103080430368517E-2</v>
+        <v>-1.8513133265238901E-2</v>
       </c>
       <c r="P41" s="66">
         <f t="shared" si="14"/>
-        <v>34.992870525950067</v>
+        <v>134.97687270319446</v>
       </c>
       <c r="Q41" s="67">
         <f t="shared" si="15"/>
-        <v>0.61716072487813445</v>
+        <v>-2.4984032604080371</v>
       </c>
       <c r="R41" s="71">
         <f t="shared" si="16"/>
-        <v>1.0639966174763384</v>
+        <v>-0.56545367507605926</v>
       </c>
       <c r="S41" s="72">
         <f t="shared" si="17"/>
-        <v>19.53485298504166</v>
+        <v>113.68445466289337</v>
       </c>
       <c r="T41" s="73">
         <f t="shared" si="18"/>
-        <v>20.265308060058818</v>
+        <v>-72.116166324133829</v>
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
@@ -5196,15 +5196,15 @@
       </c>
       <c r="C42" s="79">
         <f t="shared" si="1"/>
-        <v>2.5261129449194057</v>
+        <v>2.5949554380450901</v>
       </c>
       <c r="D42" s="76">
         <f t="shared" si="2"/>
-        <v>-20</v>
+        <v>-115</v>
       </c>
       <c r="E42" s="77">
         <f t="shared" si="3"/>
-        <v>20.000000000000004</v>
+        <v>70.000000000000014</v>
       </c>
       <c r="F42" s="79">
         <f t="shared" si="4"/>
@@ -5212,35 +5212,35 @@
       </c>
       <c r="G42" s="76">
         <f t="shared" si="5"/>
-        <v>-35</v>
+        <v>-135</v>
       </c>
       <c r="H42" s="77">
         <f t="shared" si="6"/>
-        <v>5.3029658040673552E-15</v>
+        <v>1.6544315288987496E-14</v>
       </c>
       <c r="I42" s="79">
         <f t="shared" si="7"/>
-        <v>-2.5261129449194057</v>
+        <v>-2.5949554380450901</v>
       </c>
       <c r="J42" s="76">
         <f t="shared" si="8"/>
-        <v>-20</v>
+        <v>-115</v>
       </c>
       <c r="K42" s="77">
         <f t="shared" si="9"/>
-        <v>-20.000000000000004</v>
+        <v>-70.000000000000014</v>
       </c>
       <c r="L42" s="79">
         <f t="shared" si="10"/>
-        <v>-1.04089353704597</v>
+        <v>0.5469405418108203</v>
       </c>
       <c r="M42" s="76">
         <f t="shared" si="11"/>
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="N42" s="77">
         <f t="shared" si="12"/>
-        <v>-20</v>
+        <v>70.000000000000014</v>
       </c>
       <c r="O42" s="79">
         <f t="shared" si="13"/>
@@ -5248,7 +5248,7 @@
       </c>
       <c r="P42" s="76">
         <f t="shared" si="14"/>
-        <v>35</v>
+        <v>135</v>
       </c>
       <c r="Q42" s="77">
         <f t="shared" si="15"/>
@@ -5256,15 +5256,15 @@
       </c>
       <c r="R42" s="79">
         <f t="shared" si="16"/>
-        <v>1.04089353704597</v>
+        <v>-0.5469405418108203</v>
       </c>
       <c r="S42" s="76">
         <f t="shared" si="17"/>
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="T42" s="77">
         <f t="shared" si="18"/>
-        <v>20</v>
+        <v>-70.000000000000014</v>
       </c>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
@@ -5273,75 +5273,75 @@
       </c>
       <c r="C43" s="65">
         <f t="shared" si="1"/>
-        <v>2.5030098644890373</v>
+        <v>2.6134685713103289</v>
       </c>
       <c r="D43" s="66">
         <f t="shared" si="2"/>
-        <v>-19.53043143267238</v>
+        <v>-116.27613181094999</v>
       </c>
       <c r="E43" s="67">
         <f t="shared" si="3"/>
-        <v>20.648058378833856</v>
+        <v>67.858388898528361</v>
       </c>
       <c r="F43" s="71">
         <f t="shared" si="4"/>
-        <v>3.1184895731594247</v>
+        <v>3.160105786855032</v>
       </c>
       <c r="G43" s="72">
         <f t="shared" si="5"/>
-        <v>-34.988448973580795</v>
+        <v>-134.97685924436081</v>
       </c>
       <c r="H43" s="73">
         <f t="shared" si="6"/>
-        <v>0.99991104365317329</v>
+        <v>-2.4998571957374991</v>
       </c>
       <c r="I43" s="65">
         <f t="shared" si="7"/>
-        <v>-2.5492160253497742</v>
+        <v>-2.5764423047798513</v>
       </c>
       <c r="J43" s="66">
         <f t="shared" si="8"/>
-        <v>-20.454472443261693</v>
+        <v>-113.68444120405972</v>
       </c>
       <c r="K43" s="67">
         <f t="shared" si="9"/>
-        <v>-19.341267049469508</v>
+        <v>-72.117620259463308</v>
       </c>
       <c r="L43" s="71">
         <f t="shared" si="10"/>
-        <v>-1.0639966174763384</v>
+        <v>0.56545367507605926</v>
       </c>
       <c r="M43" s="72">
         <f t="shared" si="11"/>
-        <v>19.53485298504166</v>
+        <v>113.68445466289337</v>
       </c>
       <c r="N43" s="73">
         <f t="shared" si="12"/>
-        <v>-20.265308060058818</v>
+        <v>72.116166324133829</v>
       </c>
       <c r="O43" s="65">
         <f t="shared" si="13"/>
-        <v>-2.3103080430368544E-2</v>
+        <v>1.8513133265238922E-2</v>
       </c>
       <c r="P43" s="66">
         <f t="shared" si="14"/>
-        <v>34.992870525950067</v>
+        <v>134.97687270319446</v>
       </c>
       <c r="Q43" s="67">
         <f t="shared" si="15"/>
-        <v>-0.61716072487813523</v>
+        <v>2.4984032604080402</v>
       </c>
       <c r="R43" s="71">
         <f t="shared" si="16"/>
-        <v>1.0177904566156015</v>
+        <v>-0.52842740854558135</v>
       </c>
       <c r="S43" s="72">
         <f t="shared" si="17"/>
-        <v>20.458893995630973</v>
+        <v>116.27614526978367</v>
       </c>
       <c r="T43" s="73">
         <f t="shared" si="18"/>
-        <v>19.724017368244535</v>
+        <v>-67.859842833857826</v>
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
@@ -5350,75 +5350,75 @@
       </c>
       <c r="C44" s="65">
         <f t="shared" si="1"/>
-        <v>2.4799067840586688</v>
+        <v>2.6319817045755678</v>
       </c>
       <c r="D44" s="66">
         <f t="shared" si="2"/>
-        <v>-19.046017363445763</v>
+        <v>-117.51239927295748</v>
       </c>
       <c r="E44" s="67">
         <f t="shared" si="3"/>
-        <v>21.285096298689638</v>
+        <v>65.693520941528021</v>
       </c>
       <c r="F44" s="71">
         <f t="shared" si="4"/>
-        <v>3.0953864927290562</v>
+        <v>3.1786189201202708</v>
       </c>
       <c r="G44" s="72">
         <f t="shared" si="5"/>
-        <v>-34.953802059436164</v>
+        <v>-134.90744490838915</v>
       </c>
       <c r="H44" s="73">
         <f t="shared" si="6"/>
-        <v>1.9992884062000542</v>
+        <v>-4.9988576246317802</v>
       </c>
       <c r="I44" s="65">
         <f t="shared" si="7"/>
-        <v>-2.5723191057801427</v>
+        <v>-2.5579291715146124</v>
       </c>
       <c r="J44" s="66">
         <f t="shared" si="8"/>
-        <v>-20.893606197523482</v>
+        <v>-112.32990629974668</v>
       </c>
       <c r="K44" s="67">
         <f t="shared" si="9"/>
-        <v>-18.67221111184783</v>
+        <v>-74.210523912731404</v>
       </c>
       <c r="L44" s="71">
         <f t="shared" si="10"/>
-        <v>-1.0870996979067069</v>
+        <v>0.5839668083412981</v>
       </c>
       <c r="M44" s="72">
         <f t="shared" si="11"/>
-        <v>19.063701213013974</v>
+        <v>112.32996013046863</v>
       </c>
       <c r="N44" s="73">
         <f t="shared" si="12"/>
-        <v>-20.519799945925545</v>
+        <v>74.207616540374318</v>
       </c>
       <c r="O44" s="65">
         <f t="shared" si="13"/>
-        <v>-4.6206160860737033E-2</v>
+        <v>3.7026266530477803E-2</v>
       </c>
       <c r="P44" s="66">
         <f t="shared" si="14"/>
-        <v>34.971485909004379</v>
+        <v>134.90749873911111</v>
       </c>
       <c r="Q44" s="67">
         <f t="shared" si="15"/>
-        <v>-1.2339920534359656</v>
+        <v>4.9959502522747368</v>
       </c>
       <c r="R44" s="71">
         <f t="shared" si="16"/>
-        <v>0.99468737618523295</v>
+        <v>-0.5099142752803425</v>
       </c>
       <c r="S44" s="72">
         <f t="shared" si="17"/>
-        <v>20.911290047091697</v>
+        <v>117.51245310367943</v>
       </c>
       <c r="T44" s="73">
         <f t="shared" si="18"/>
-        <v>19.437507464611908</v>
+        <v>-65.696428313885079</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
@@ -5427,75 +5427,75 @@
       </c>
       <c r="C45" s="65">
         <f t="shared" si="1"/>
-        <v>2.4568037036283004</v>
+        <v>2.6504948378408066</v>
       </c>
       <c r="D45" s="66">
         <f t="shared" si="2"/>
-        <v>-18.547016337955782</v>
+        <v>-118.70837868463155</v>
       </c>
       <c r="E45" s="67">
         <f t="shared" si="3"/>
-        <v>21.910773754219893</v>
+        <v>63.506138086215103</v>
       </c>
       <c r="F45" s="71">
         <f t="shared" si="4"/>
-        <v>3.0722834122986877</v>
+        <v>3.1971320533855097</v>
       </c>
       <c r="G45" s="72">
         <f t="shared" si="5"/>
-        <v>-34.896077749614562</v>
+        <v>-134.79178078220454</v>
       </c>
       <c r="H45" s="73">
         <f t="shared" si="6"/>
-        <v>2.9975986913752215</v>
+        <v>-7.4961448134761355</v>
       </c>
       <c r="I45" s="65">
         <f t="shared" si="7"/>
-        <v>-2.5954221862105111</v>
+        <v>-2.5394160382493736</v>
       </c>
       <c r="J45" s="66">
         <f t="shared" si="8"/>
-        <v>-21.317166884548143</v>
+        <v>-110.93685952181639</v>
       </c>
       <c r="K45" s="67">
         <f t="shared" si="9"/>
-        <v>-17.993189281413734</v>
+        <v>-76.277993666648783</v>
       </c>
       <c r="L45" s="71">
         <f t="shared" si="10"/>
-        <v>-1.1102027783370756</v>
+        <v>0.60247994160653706</v>
       </c>
       <c r="M45" s="72">
         <f t="shared" si="11"/>
-        <v>18.586796151085473</v>
+        <v>110.93698062364474</v>
       </c>
       <c r="N45" s="73">
         <f t="shared" si="12"/>
-        <v>-20.763339828006092</v>
+        <v>76.273633853697149</v>
       </c>
       <c r="O45" s="65">
         <f t="shared" si="13"/>
-        <v>-6.9309241291105578E-2</v>
+        <v>5.5539399795716732E-2</v>
       </c>
       <c r="P45" s="66">
         <f t="shared" si="14"/>
-        <v>34.93585756274426</v>
+        <v>134.79190188403288</v>
       </c>
       <c r="Q45" s="67">
         <f t="shared" si="15"/>
-        <v>-1.8501647651614226</v>
+        <v>7.4917850005245246</v>
       </c>
       <c r="R45" s="71">
         <f t="shared" si="16"/>
-        <v>0.97158429575486438</v>
+        <v>-0.49140114201510354</v>
       </c>
       <c r="S45" s="72">
         <f t="shared" si="17"/>
-        <v>21.356946697677845</v>
+        <v>118.70849978645992</v>
       </c>
       <c r="T45" s="73">
         <f t="shared" si="18"/>
-        <v>19.140623207627524</v>
+        <v>-63.510497899166715</v>
       </c>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
@@ -5504,75 +5504,75 @@
       </c>
       <c r="C46" s="65">
         <f t="shared" si="1"/>
-        <v>2.4337006231979315</v>
+        <v>2.6690079711060459</v>
       </c>
       <c r="D46" s="66">
         <f t="shared" si="2"/>
-        <v>-18.033694687313591</v>
+        <v>-119.86366015235637</v>
       </c>
       <c r="E46" s="67">
         <f t="shared" si="3"/>
-        <v>22.524756803481743</v>
+        <v>61.296990006253715</v>
       </c>
       <c r="F46" s="71">
         <f t="shared" si="4"/>
-        <v>3.0491803318683193</v>
+        <v>3.2156451866507485</v>
       </c>
       <c r="G46" s="72">
         <f t="shared" si="5"/>
-        <v>-34.81530685323019</v>
+        <v>-134.62990650694664</v>
       </c>
       <c r="H46" s="73">
         <f t="shared" si="6"/>
-        <v>3.9943090724429466</v>
+        <v>-9.990862876236319</v>
       </c>
       <c r="I46" s="65">
         <f t="shared" si="7"/>
-        <v>-2.61852526664088</v>
+        <v>-2.5209029049841343</v>
       </c>
       <c r="J46" s="66">
         <f t="shared" si="8"/>
-        <v>-21.724928437889609</v>
+        <v>-109.50577830405679</v>
       </c>
       <c r="K46" s="67">
         <f t="shared" si="9"/>
-        <v>-17.304563971527834</v>
+        <v>-78.319320944926616</v>
       </c>
       <c r="L46" s="71">
         <f t="shared" si="10"/>
-        <v>-1.1333058587674441</v>
+        <v>0.62099307487177591</v>
       </c>
       <c r="M46" s="72">
         <f t="shared" si="11"/>
-        <v>18.104392337119965</v>
+        <v>109.50599355315411</v>
       </c>
       <c r="N46" s="73">
         <f t="shared" si="12"/>
-        <v>-20.995797722103841</v>
+        <v>78.313510185602979</v>
       </c>
       <c r="O46" s="65">
         <f t="shared" si="13"/>
-        <v>-9.2412321721474067E-2</v>
+        <v>7.4052533060955605E-2</v>
       </c>
       <c r="P46" s="66">
         <f t="shared" si="14"/>
-        <v>34.886004503036553</v>
+        <v>134.63012175604393</v>
       </c>
       <c r="Q46" s="67">
         <f t="shared" si="15"/>
-        <v>-2.4653499910650618</v>
+        <v>9.98505211691276</v>
       </c>
       <c r="R46" s="71">
         <f t="shared" si="16"/>
-        <v>0.94848121532449592</v>
+        <v>-0.4728880087498647</v>
       </c>
       <c r="S46" s="72">
         <f t="shared" si="17"/>
-        <v>21.795626087695972</v>
+        <v>119.86387540145367</v>
       </c>
       <c r="T46" s="73">
         <f t="shared" si="18"/>
-        <v>18.833523052905722</v>
+        <v>-61.302800765577338</v>
       </c>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
@@ -5581,75 +5581,75 @@
       </c>
       <c r="C47" s="65">
         <f t="shared" si="1"/>
-        <v>2.410597542767563</v>
+        <v>2.6875211043712848</v>
       </c>
       <c r="D47" s="66">
         <f t="shared" si="2"/>
-        <v>-17.506326385957379</v>
+        <v>-120.97784773077237</v>
       </c>
       <c r="E47" s="67">
         <f t="shared" si="3"/>
-        <v>23.126717746171163</v>
+        <v>59.066833834823406</v>
       </c>
       <c r="F47" s="71">
         <f t="shared" si="4"/>
-        <v>3.0260772514379504</v>
+        <v>3.2341583199159878</v>
       </c>
       <c r="G47" s="72">
         <f t="shared" si="5"/>
-        <v>-34.711532480019251</v>
+        <v>-134.42187756118923</v>
       </c>
       <c r="H47" s="73">
         <f t="shared" si="6"/>
-        <v>4.9888875765820719</v>
+        <v>-12.482156807385259</v>
       </c>
       <c r="I47" s="65">
         <f t="shared" si="7"/>
-        <v>-2.6416283470712485</v>
+        <v>-2.5023897717188954</v>
       </c>
       <c r="J47" s="66">
         <f t="shared" si="8"/>
-        <v>-22.116673223551054</v>
+        <v>-108.03715311565934</v>
       </c>
       <c r="K47" s="67">
         <f t="shared" si="9"/>
-        <v>-16.606702721202282</v>
+        <v>-80.33380613099024</v>
       </c>
       <c r="L47" s="71">
         <f t="shared" si="10"/>
-        <v>-1.1564089391978125</v>
+        <v>0.63950620813701486</v>
       </c>
       <c r="M47" s="72">
         <f t="shared" si="11"/>
-        <v>17.616747243822388</v>
+        <v>108.03748935592138</v>
       </c>
       <c r="N47" s="73">
         <f t="shared" si="12"/>
-        <v>-21.217049558795946</v>
+        <v>80.326546416794784</v>
       </c>
       <c r="O47" s="65">
         <f t="shared" si="13"/>
-        <v>-0.11551540215184261</v>
+        <v>9.2565666326194534E-2</v>
       </c>
       <c r="P47" s="66">
         <f t="shared" si="14"/>
-        <v>34.821953337884253</v>
+        <v>134.42221380145125</v>
       </c>
       <c r="Q47" s="67">
         <f t="shared" si="15"/>
-        <v>-3.0792193892068549</v>
+        <v>12.474897093189828</v>
       </c>
       <c r="R47" s="71">
         <f t="shared" si="16"/>
-        <v>0.92537813489412735</v>
+        <v>-0.45437487548462574</v>
       </c>
       <c r="S47" s="72">
         <f t="shared" si="17"/>
-        <v>22.227094081416055</v>
+        <v>120.9781839710344</v>
       </c>
       <c r="T47" s="73">
         <f t="shared" si="18"/>
-        <v>18.516370908577485</v>
+        <v>-59.074093549018841</v>
       </c>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
@@ -5658,75 +5658,75 @@
       </c>
       <c r="C48" s="65">
         <f t="shared" si="1"/>
-        <v>2.3874944623371945</v>
+        <v>2.7060342376365236</v>
       </c>
       <c r="D48" s="66">
         <f t="shared" si="2"/>
-        <v>-16.965192905424296</v>
+        <v>-122.05055955847723</v>
       </c>
       <c r="E48" s="67">
         <f t="shared" si="3"/>
-        <v>23.716335298526101</v>
+        <v>56.816433905129294</v>
       </c>
       <c r="F48" s="71">
         <f t="shared" si="4"/>
-        <v>3.0029741710075819</v>
+        <v>3.2526714531812266</v>
       </c>
       <c r="G48" s="72">
         <f t="shared" si="5"/>
-        <v>-34.584810017331115</v>
+        <v>-134.16776524192619</v>
       </c>
       <c r="H48" s="73">
         <f t="shared" si="6"/>
-        <v>5.9808033688150415</v>
+        <v>-14.96917277493572</v>
       </c>
       <c r="I48" s="65">
         <f t="shared" si="7"/>
-        <v>-2.664731427501617</v>
+        <v>-2.4838766384536566</v>
       </c>
       <c r="J48" s="66">
         <f t="shared" si="8"/>
-        <v>-22.492192156142416</v>
+        <v>-106.53148729312204</v>
       </c>
       <c r="K48" s="67">
         <f t="shared" si="9"/>
-        <v>-15.899977998934611</v>
+        <v>-82.32075880775642</v>
       </c>
       <c r="L48" s="71">
         <f t="shared" si="10"/>
-        <v>-1.1795120196281812</v>
+        <v>0.65801934140225371</v>
       </c>
       <c r="M48" s="72">
         <f t="shared" si="11"/>
-        <v>17.124121141318291</v>
+        <v>106.53197132697777</v>
       </c>
       <c r="N48" s="73">
         <f t="shared" si="12"/>
-        <v>-21.426977249652715</v>
+        <v>82.312052626784237</v>
       </c>
       <c r="O48" s="65">
         <f t="shared" si="13"/>
-        <v>-0.13861848258221116</v>
+        <v>0.11107879959143346</v>
       </c>
       <c r="P48" s="66">
         <f t="shared" si="14"/>
-        <v>34.743738253225104</v>
+        <v>134.1682492757819</v>
       </c>
       <c r="Q48" s="67">
         <f t="shared" si="15"/>
-        <v>-3.6914453199416584</v>
+        <v>14.960466593963563</v>
       </c>
       <c r="R48" s="71">
         <f t="shared" si="16"/>
-        <v>0.90227505446375877</v>
+        <v>-0.43586174221938684</v>
       </c>
       <c r="S48" s="72">
         <f t="shared" si="17"/>
-        <v>22.651120392036404</v>
+        <v>122.05104359233296</v>
       </c>
       <c r="T48" s="73">
         <f t="shared" si="18"/>
-        <v>18.189336047807981</v>
+        <v>-56.825140086101456</v>
       </c>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
@@ -5735,75 +5735,75 @@
       </c>
       <c r="C49" s="65">
         <f t="shared" si="1"/>
-        <v>2.3643913819068261</v>
+        <v>2.7245473709017625</v>
       </c>
       <c r="D49" s="66">
         <f t="shared" si="2"/>
-        <v>-16.410583064121127</v>
+        <v>-123.08142798889988</v>
       </c>
       <c r="E49" s="67">
         <f t="shared" si="3"/>
-        <v>24.293294764804742</v>
+        <v>54.546561488445221</v>
       </c>
       <c r="F49" s="71">
         <f t="shared" si="4"/>
-        <v>2.9798710905772134</v>
+        <v>3.2711845864464655</v>
       </c>
       <c r="G49" s="72">
         <f t="shared" si="5"/>
-        <v>-34.435207100566458</v>
+        <v>-133.86765664013612</v>
       </c>
       <c r="H49" s="73">
         <f t="shared" si="6"/>
-        <v>6.9695270353298122</v>
+        <v>-17.451058413071326</v>
       </c>
       <c r="I49" s="65">
         <f t="shared" si="7"/>
-        <v>-2.6878345079319854</v>
+        <v>-2.4653635051884177</v>
       </c>
       <c r="J49" s="66">
         <f t="shared" si="8"/>
-        <v>-22.851284810475221</v>
+        <v>-104.98929686774301</v>
       </c>
       <c r="K49" s="67">
         <f t="shared" si="9"/>
-        <v>-15.184767003910704</v>
+        <v>-84.279497994257369</v>
       </c>
       <c r="L49" s="71">
         <f t="shared" si="10"/>
-        <v>-1.2026151000585497</v>
+        <v>0.67653247466749267</v>
       </c>
       <c r="M49" s="72">
         <f t="shared" si="11"/>
-        <v>16.626776958240217</v>
+        <v>104.98995544696859</v>
       </c>
       <c r="N49" s="73">
         <f t="shared" si="12"/>
-        <v>-21.625468750264794</v>
+        <v>84.269348330345778</v>
       </c>
       <c r="O49" s="65">
         <f t="shared" si="13"/>
-        <v>-0.16172156301257964</v>
+        <v>0.12959193285667234</v>
       </c>
       <c r="P49" s="66">
         <f t="shared" si="14"/>
-        <v>34.651400994685552</v>
+        <v>133.86831521936168</v>
       </c>
       <c r="Q49" s="67">
         <f t="shared" si="15"/>
-        <v>-4.3017010207898609</v>
+        <v>17.440908749159757</v>
       </c>
       <c r="R49" s="71">
         <f t="shared" si="16"/>
-        <v>0.87917197403339031</v>
+        <v>-0.41734860895414794</v>
       </c>
       <c r="S49" s="72">
         <f t="shared" si="17"/>
-        <v>23.067478704594315</v>
+        <v>123.08208656812548</v>
       </c>
       <c r="T49" s="73">
         <f t="shared" si="18"/>
-        <v>17.852593018450641</v>
+        <v>-54.556711152356797</v>
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
@@ -5812,75 +5812,75 @@
       </c>
       <c r="C50" s="65">
         <f t="shared" si="1"/>
-        <v>2.3412883014764576</v>
+        <v>2.7430605041670013</v>
       </c>
       <c r="D50" s="66">
         <f t="shared" si="2"/>
-        <v>-15.842792873173584</v>
+        <v>-124.07009971630248</v>
       </c>
       <c r="E50" s="67">
         <f t="shared" si="3"/>
-        <v>24.857288205247652</v>
+        <v>52.257994529778742</v>
       </c>
       <c r="F50" s="71">
         <f t="shared" si="4"/>
-        <v>2.956768010146845</v>
+        <v>3.2896977197117043</v>
       </c>
       <c r="G50" s="72">
         <f t="shared" si="5"/>
-        <v>-34.26280357707833</v>
+        <v>-133.52165461093401</v>
       </c>
       <c r="H50" s="73">
         <f t="shared" si="6"/>
-        <v>7.9545308660430658</v>
+        <v>-19.926963114274553</v>
       </c>
       <c r="I50" s="65">
         <f t="shared" si="7"/>
-        <v>-2.7109375883623539</v>
+        <v>-2.4468503719231789</v>
       </c>
       <c r="J50" s="66">
         <f t="shared" si="8"/>
-        <v>-23.19375952853526</v>
+        <v>-103.41111038876282</v>
       </c>
       <c r="K50" s="67">
         <f t="shared" si="9"/>
-        <v>-14.461451464682787</v>
+        <v>-86.209352379030832</v>
       </c>
       <c r="L50" s="71">
         <f t="shared" si="10"/>
-        <v>-1.2257181804889181</v>
+        <v>0.69504560793273162</v>
       </c>
       <c r="M50" s="72">
         <f t="shared" si="11"/>
-        <v>16.124980141395174</v>
+        <v>103.41197020531315</v>
       </c>
       <c r="N50" s="73">
         <f t="shared" si="12"/>
-        <v>-21.812418120044455</v>
+        <v>86.197762710736725</v>
       </c>
       <c r="O50" s="65">
         <f t="shared" si="13"/>
-        <v>-0.18482464344294819</v>
+        <v>0.14810506612191127</v>
       </c>
       <c r="P50" s="66">
         <f t="shared" si="14"/>
-        <v>34.544990845299921</v>
+        <v>133.52251442748434</v>
       </c>
       <c r="Q50" s="67">
         <f t="shared" si="15"/>
-        <v>-4.909660780839868</v>
+        <v>19.915373445980478</v>
       </c>
       <c r="R50" s="71">
         <f t="shared" si="16"/>
-        <v>0.85606889360302185</v>
+        <v>-0.39883547568890904</v>
       </c>
       <c r="S50" s="72">
         <f t="shared" si="17"/>
-        <v>23.475946796756844</v>
+        <v>124.07095953285281</v>
       </c>
       <c r="T50" s="73">
         <f t="shared" si="18"/>
-        <v>17.506321549885975</v>
+        <v>-52.26958419807282</v>
       </c>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
@@ -5889,75 +5889,75 @@
       </c>
       <c r="C51" s="65">
         <f t="shared" si="1"/>
-        <v>2.3181852210460892</v>
+        <v>2.7615736374322402</v>
       </c>
       <c r="D51" s="66">
         <f t="shared" si="2"/>
-        <v>-15.262125378436776</v>
+        <v>-125.01623589686776</v>
       </c>
       <c r="E51" s="67">
         <f t="shared" si="3"/>
-        <v>25.408014600434004</v>
+        <v>49.951517381248848</v>
       </c>
       <c r="F51" s="71">
         <f t="shared" si="4"/>
-        <v>2.9336649297164765</v>
+        <v>3.3082108529769432</v>
       </c>
       <c r="G51" s="72">
         <f t="shared" si="5"/>
-        <v>-34.067691463555342</v>
+        <v>-133.12987773832018</v>
       </c>
       <c r="H51" s="73">
         <f t="shared" si="6"/>
-        <v>8.9352891362541804</v>
+        <v>-22.39603832085233</v>
       </c>
       <c r="I51" s="65">
         <f t="shared" si="7"/>
-        <v>-2.7340406687927223</v>
+        <v>-2.42833723865794</v>
       </c>
       <c r="J51" s="66">
         <f t="shared" si="8"/>
-        <v>-23.519433521775909</v>
+        <v>-101.79746874221689</v>
       </c>
       <c r="K51" s="67">
         <f t="shared" si="9"/>
-        <v>-13.730417435430004</v>
+        <v>-88.109660550196153</v>
       </c>
       <c r="L51" s="71">
         <f t="shared" si="10"/>
-        <v>-1.2488212609192866</v>
+        <v>0.71355874119797047</v>
       </c>
       <c r="M51" s="72">
         <f t="shared" si="11"/>
-        <v>15.618998514088089</v>
+        <v>101.79855641907753</v>
       </c>
       <c r="N51" s="73">
         <f t="shared" si="12"/>
-        <v>-21.98772557876913</v>
+        <v>88.096634849603845</v>
       </c>
       <c r="O51" s="65">
         <f t="shared" si="13"/>
-        <v>-0.20792772387331668</v>
+        <v>0.16661819938715014</v>
       </c>
       <c r="P51" s="66">
         <f t="shared" si="14"/>
-        <v>34.424564599206647</v>
+        <v>133.13096541518081</v>
       </c>
       <c r="Q51" s="67">
         <f t="shared" si="15"/>
-        <v>-5.5150001145893075</v>
+        <v>22.383012620260047</v>
       </c>
       <c r="R51" s="71">
         <f t="shared" si="16"/>
-        <v>0.83296581317265328</v>
+        <v>-0.38032234242367013</v>
       </c>
       <c r="S51" s="72">
         <f t="shared" si="17"/>
-        <v>23.876306657427222</v>
+        <v>125.01732357372842</v>
       </c>
       <c r="T51" s="73">
         <f t="shared" si="18"/>
-        <v>17.150706457094863</v>
+        <v>-49.964543081841143</v>
       </c>
     </row>
     <row r="52" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5966,79 +5966,111 @@
       </c>
       <c r="C52" s="88">
         <f t="shared" si="1"/>
-        <v>2.2950821406157207</v>
+        <v>2.780086770697479</v>
       </c>
       <c r="D52" s="89">
         <f t="shared" si="2"/>
-        <v>-14.668890498750928</v>
+        <v>-125.91951226482961</v>
       </c>
       <c r="E52" s="90">
         <f t="shared" si="3"/>
-        <v>25.945180011944267</v>
+        <v>47.62792053326794</v>
       </c>
       <c r="F52" s="91">
         <f t="shared" si="4"/>
-        <v>2.9105618492861081</v>
+        <v>3.326723986242182</v>
       </c>
       <c r="G52" s="92">
         <f t="shared" si="5"/>
-        <v>-33.849974896909728</v>
+        <v>-132.69246029453819</v>
       </c>
       <c r="H52" s="93">
         <f t="shared" si="6"/>
-        <v>9.9112783872395323</v>
+        <v>-24.857437815759127</v>
       </c>
       <c r="I52" s="88">
         <f t="shared" si="7"/>
-        <v>-2.7571437492230908</v>
+        <v>-2.4098241053927012</v>
       </c>
       <c r="J52" s="89">
         <f t="shared" si="8"/>
-        <v>-23.82813296867765</v>
+        <v>-100.14892496555947</v>
       </c>
       <c r="K52" s="90">
         <f t="shared" si="9"/>
-        <v>-12.992055089910252</v>
+        <v>-89.979771222137614</v>
       </c>
       <c r="L52" s="91">
         <f t="shared" si="10"/>
-        <v>-1.2719243413496553</v>
+        <v>0.73207187446320932</v>
       </c>
       <c r="M52" s="92">
         <f t="shared" si="11"/>
-        <v>15.109102133176851</v>
+        <v>100.15026704762228</v>
       </c>
       <c r="N52" s="93">
         <f t="shared" si="12"/>
-        <v>-22.151297559836966</v>
+        <v>89.965313953497443</v>
       </c>
       <c r="O52" s="88">
         <f t="shared" si="13"/>
-        <v>-0.23103080430368522</v>
+        <v>0.18513133265238907</v>
       </c>
       <c r="P52" s="89">
         <f t="shared" si="14"/>
-        <v>34.29018653133565</v>
+        <v>132.69380237660101</v>
       </c>
       <c r="Q52" s="90">
         <f t="shared" si="15"/>
-        <v>-6.1173959351322393</v>
+        <v>24.842980547118994</v>
       </c>
       <c r="R52" s="91">
         <f t="shared" si="16"/>
-        <v>0.80986273274228471</v>
+        <v>-0.36180920915843123</v>
       </c>
       <c r="S52" s="92">
         <f t="shared" si="17"/>
-        <v>24.268344603103579</v>
+        <v>125.92085434689243</v>
       </c>
       <c r="T52" s="93">
         <f t="shared" si="18"/>
-        <v>16.785937542017532</v>
+        <v>-47.642377801908076</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G12:M12"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="G26:M26"/>
+    <mergeCell ref="G13:M18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="G19:M24"/>
     <mergeCell ref="B29:T29"/>
@@ -6055,38 +6087,6 @@
     <mergeCell ref="R30:T30"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:M25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="G26:M26"/>
-    <mergeCell ref="G13:M18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G12:M12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>